<commit_message>
deuxième partie du modèle, à compléter
</commit_message>
<xml_diff>
--- a/base_de_données_v1.xlsx
+++ b/base_de_données_v1.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
Ajout du df sur potential growth (voir notebook : "test données_copie_alt"). Il manque convertir les données annuelles en trimestrielles.
</commit_message>
<xml_diff>
--- a/base_de_données_v1.xlsx
+++ b/base_de_données_v1.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
fin construction du df sur le potential growth (voir le notebook "copie_alternative"), si vous pensez que c'est bon, vous pouvez l'ajouter au notebook principal
</commit_message>
<xml_diff>
--- a/base_de_données_v1.xlsx
+++ b/base_de_données_v1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:EK121"/>
+  <dimension ref="A1:EK124"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1156,9 +1156,7 @@
       <c r="E2" t="n">
         <v>5.043334</v>
       </c>
-      <c r="F2" t="n">
-        <v>40</v>
-      </c>
+      <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="n">
         <v>53331.5</v>
@@ -1169,9 +1167,7 @@
       <c r="J2" t="n">
         <v>5.706666</v>
       </c>
-      <c r="K2" t="n">
-        <v>37.8</v>
-      </c>
+      <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="n">
         <v>3175.8</v>
@@ -1198,9 +1194,7 @@
       <c r="Y2" t="n">
         <v>6.49543</v>
       </c>
-      <c r="Z2" t="n">
-        <v>34.3</v>
-      </c>
+      <c r="Z2" t="inlineStr"/>
       <c r="AA2" t="inlineStr"/>
       <c r="AB2" t="n">
         <v>647.2</v>
@@ -1218,9 +1212,7 @@
       <c r="AI2" t="n">
         <v>5.966667</v>
       </c>
-      <c r="AJ2" t="n">
-        <v>36.9</v>
-      </c>
+      <c r="AJ2" t="inlineStr"/>
       <c r="AK2" t="inlineStr"/>
       <c r="AL2" t="n">
         <v>302514.4</v>
@@ -1231,9 +1223,7 @@
       <c r="AN2" t="n">
         <v>6.600767</v>
       </c>
-      <c r="AO2" t="n">
-        <v>39.7</v>
-      </c>
+      <c r="AO2" t="inlineStr"/>
       <c r="AP2" t="inlineStr"/>
       <c r="AQ2" t="n">
         <v>476161.9</v>
@@ -1244,9 +1234,7 @@
       <c r="AS2" t="n">
         <v>5.11</v>
       </c>
-      <c r="AT2" t="n">
-        <v>38.7</v>
-      </c>
+      <c r="AT2" t="inlineStr"/>
       <c r="AU2" t="inlineStr"/>
       <c r="AV2" t="n">
         <v>24031.8</v>
@@ -1255,9 +1243,7 @@
       <c r="AX2" t="n">
         <v>18.11684</v>
       </c>
-      <c r="AY2" t="n">
-        <v>42.3</v>
-      </c>
+      <c r="AY2" t="inlineStr"/>
       <c r="AZ2" t="inlineStr"/>
       <c r="BA2" t="n">
         <v>8738.4</v>
@@ -1277,9 +1263,7 @@
       <c r="BH2" t="n">
         <v>6.65</v>
       </c>
-      <c r="BI2" t="n">
-        <v>41.2</v>
-      </c>
+      <c r="BI2" t="inlineStr"/>
       <c r="BJ2" t="inlineStr"/>
       <c r="BK2" t="n">
         <v>12803</v>
@@ -1290,9 +1274,7 @@
       <c r="BM2" t="n">
         <v>6.523334</v>
       </c>
-      <c r="BN2" t="n">
-        <v>39.6</v>
-      </c>
+      <c r="BN2" t="inlineStr"/>
       <c r="BO2" t="inlineStr"/>
       <c r="BP2" t="n">
         <v>211263.5</v>
@@ -1303,9 +1285,7 @@
       <c r="BR2" t="n">
         <v>9.743333</v>
       </c>
-      <c r="BS2" t="n">
-        <v>39.3</v>
-      </c>
+      <c r="BS2" t="inlineStr"/>
       <c r="BT2" t="inlineStr"/>
       <c r="BU2" t="n">
         <v>930.2</v>
@@ -1328,9 +1308,7 @@
         <v>7.781</v>
       </c>
       <c r="CG2" t="inlineStr"/>
-      <c r="CH2" t="n">
-        <v>39.7</v>
-      </c>
+      <c r="CH2" t="inlineStr"/>
       <c r="CI2" t="inlineStr"/>
       <c r="CJ2" t="n">
         <v>83633</v>
@@ -1341,9 +1319,7 @@
       <c r="CL2" t="n">
         <v>5.13</v>
       </c>
-      <c r="CM2" t="n">
-        <v>30.5</v>
-      </c>
+      <c r="CM2" t="inlineStr"/>
       <c r="CN2" t="inlineStr"/>
       <c r="CO2" t="n">
         <v>28755.9</v>
@@ -1354,9 +1330,7 @@
       <c r="CQ2" t="n">
         <v>5.536667</v>
       </c>
-      <c r="CR2" t="n">
-        <v>34.4</v>
-      </c>
+      <c r="CR2" t="inlineStr"/>
       <c r="CS2" t="inlineStr"/>
       <c r="CT2" t="n">
         <v>25719.3</v>
@@ -1376,9 +1350,7 @@
       <c r="DA2" t="n">
         <v>10.527</v>
       </c>
-      <c r="DB2" t="n">
-        <v>41.6</v>
-      </c>
+      <c r="DB2" t="inlineStr"/>
       <c r="DC2" t="inlineStr"/>
       <c r="DD2" t="n">
         <v>6370.1</v>
@@ -1410,9 +1382,7 @@
       <c r="DU2" t="n">
         <v>9.032666000000001</v>
       </c>
-      <c r="DV2" t="n">
-        <v>38.3</v>
-      </c>
+      <c r="DV2" t="inlineStr"/>
       <c r="DW2" t="inlineStr"/>
       <c r="DX2" t="n">
         <v>49061.2</v>
@@ -1423,9 +1393,7 @@
       <c r="DZ2" t="n">
         <v>8.196667</v>
       </c>
-      <c r="EA2" t="n">
-        <v>34</v>
-      </c>
+      <c r="EA2" t="inlineStr"/>
       <c r="EB2" t="inlineStr"/>
       <c r="EC2" t="n">
         <v>64546.7</v>
@@ -1445,9 +1413,7 @@
       <c r="EJ2" t="n">
         <v>6.72241</v>
       </c>
-      <c r="EK2" t="n">
-        <v>36.9</v>
-      </c>
+      <c r="EK2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -1465,9 +1431,7 @@
       <c r="E3" t="n">
         <v>4.68</v>
       </c>
-      <c r="F3" t="n">
-        <v>39.95</v>
-      </c>
+      <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="n">
         <v>56119.3</v>
@@ -1478,9 +1442,7 @@
       <c r="J3" t="n">
         <v>5.05</v>
       </c>
-      <c r="K3" t="n">
-        <v>37.8</v>
-      </c>
+      <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr"/>
       <c r="M3" t="n">
         <v>3162.8</v>
@@ -1507,9 +1469,7 @@
       <c r="Y3" t="n">
         <v>6.854634</v>
       </c>
-      <c r="Z3" t="n">
-        <v>34.22499999999999</v>
-      </c>
+      <c r="Z3" t="inlineStr"/>
       <c r="AA3" t="inlineStr"/>
       <c r="AB3" t="n">
         <v>766.7</v>
@@ -1527,9 +1487,7 @@
       <c r="AI3" t="n">
         <v>5.953333</v>
       </c>
-      <c r="AJ3" t="n">
-        <v>37.075</v>
-      </c>
+      <c r="AJ3" t="inlineStr"/>
       <c r="AK3" t="inlineStr"/>
       <c r="AL3" t="n">
         <v>305681.9</v>
@@ -1540,9 +1498,7 @@
       <c r="AN3" t="n">
         <v>7.4825</v>
       </c>
-      <c r="AO3" t="n">
-        <v>39.675</v>
-      </c>
+      <c r="AO3" t="inlineStr"/>
       <c r="AP3" t="inlineStr"/>
       <c r="AQ3" t="n">
         <v>491129.7</v>
@@ -1553,9 +1509,7 @@
       <c r="AS3" t="n">
         <v>4.6</v>
       </c>
-      <c r="AT3" t="n">
-        <v>38.7</v>
-      </c>
+      <c r="AT3" t="inlineStr"/>
       <c r="AU3" t="inlineStr"/>
       <c r="AV3" t="n">
         <v>24618.7</v>
@@ -1564,9 +1518,7 @@
       <c r="AX3" t="n">
         <v>16.46729</v>
       </c>
-      <c r="AY3" t="n">
-        <v>42.2</v>
-      </c>
+      <c r="AY3" t="inlineStr"/>
       <c r="AZ3" t="inlineStr"/>
       <c r="BA3" t="n">
         <v>8771.5</v>
@@ -1586,9 +1538,7 @@
       <c r="BH3" t="n">
         <v>7.1</v>
       </c>
-      <c r="BI3" t="n">
-        <v>41.425</v>
-      </c>
+      <c r="BI3" t="inlineStr"/>
       <c r="BJ3" t="inlineStr"/>
       <c r="BK3" t="n">
         <v>13418.5</v>
@@ -1599,9 +1549,7 @@
       <c r="BM3" t="n">
         <v>6.73</v>
       </c>
-      <c r="BN3" t="n">
-        <v>39.725</v>
-      </c>
+      <c r="BN3" t="inlineStr"/>
       <c r="BO3" t="inlineStr"/>
       <c r="BP3" t="n">
         <v>214037.6</v>
@@ -1612,9 +1560,7 @@
       <c r="BR3" t="n">
         <v>10.78667</v>
       </c>
-      <c r="BS3" t="n">
-        <v>39.175</v>
-      </c>
+      <c r="BS3" t="inlineStr"/>
       <c r="BT3" t="inlineStr"/>
       <c r="BU3" t="n">
         <v>1022.8</v>
@@ -1637,9 +1583,7 @@
         <v>7.343</v>
       </c>
       <c r="CG3" t="inlineStr"/>
-      <c r="CH3" t="n">
-        <v>39.6</v>
-      </c>
+      <c r="CH3" t="inlineStr"/>
       <c r="CI3" t="inlineStr"/>
       <c r="CJ3" t="n">
         <v>86665.8</v>
@@ -1650,9 +1594,7 @@
       <c r="CL3" t="n">
         <v>4.486667</v>
       </c>
-      <c r="CM3" t="n">
-        <v>30.95</v>
-      </c>
+      <c r="CM3" t="inlineStr"/>
       <c r="CN3" t="inlineStr"/>
       <c r="CO3" t="n">
         <v>28112.2</v>
@@ -1663,9 +1605,7 @@
       <c r="CQ3" t="n">
         <v>5.606667</v>
       </c>
-      <c r="CR3" t="n">
-        <v>34.525</v>
-      </c>
+      <c r="CR3" t="inlineStr"/>
       <c r="CS3" t="inlineStr"/>
       <c r="CT3" t="n">
         <v>26686.2</v>
@@ -1685,9 +1625,7 @@
       <c r="DA3" t="n">
         <v>10.20033</v>
       </c>
-      <c r="DB3" t="n">
-        <v>41.4</v>
-      </c>
+      <c r="DB3" t="inlineStr"/>
       <c r="DC3" t="inlineStr"/>
       <c r="DD3" t="n">
         <v>6573.1</v>
@@ -1719,9 +1657,7 @@
       <c r="DU3" t="n">
         <v>9.454333</v>
       </c>
-      <c r="DV3" t="n">
-        <v>38.22499999999999</v>
-      </c>
+      <c r="DV3" t="inlineStr"/>
       <c r="DW3" t="inlineStr"/>
       <c r="DX3" t="n">
         <v>49347.7</v>
@@ -1732,9 +1668,7 @@
       <c r="DZ3" t="n">
         <v>8.903333999999999</v>
       </c>
-      <c r="EA3" t="n">
-        <v>34.1</v>
-      </c>
+      <c r="EA3" t="inlineStr"/>
       <c r="EB3" t="inlineStr"/>
       <c r="EC3" t="n">
         <v>67655.10000000001</v>
@@ -1754,9 +1688,7 @@
       <c r="EJ3" t="n">
         <v>6.742444</v>
       </c>
-      <c r="EK3" t="n">
-        <v>36.85</v>
-      </c>
+      <c r="EK3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -1774,9 +1706,7 @@
       <c r="E4" t="n">
         <v>4.373333</v>
       </c>
-      <c r="F4" t="n">
-        <v>39.9</v>
-      </c>
+      <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="n">
         <v>53741.7</v>
@@ -1787,9 +1717,7 @@
       <c r="J4" t="n">
         <v>4.416667</v>
       </c>
-      <c r="K4" t="n">
-        <v>37.8</v>
-      </c>
+      <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr"/>
       <c r="M4" t="n">
         <v>3796.9</v>
@@ -1816,9 +1744,7 @@
       <c r="Y4" t="n">
         <v>6.110099</v>
       </c>
-      <c r="Z4" t="n">
-        <v>34.15</v>
-      </c>
+      <c r="Z4" t="inlineStr"/>
       <c r="AA4" t="inlineStr"/>
       <c r="AB4" t="n">
         <v>764.9</v>
@@ -1836,9 +1762,7 @@
       <c r="AI4" t="n">
         <v>6.053333</v>
       </c>
-      <c r="AJ4" t="n">
-        <v>37.25</v>
-      </c>
+      <c r="AJ4" t="inlineStr"/>
       <c r="AK4" t="inlineStr"/>
       <c r="AL4" t="n">
         <v>298966.5</v>
@@ -1849,9 +1773,7 @@
       <c r="AN4" t="n">
         <v>6.122233</v>
       </c>
-      <c r="AO4" t="n">
-        <v>39.65000000000001</v>
-      </c>
+      <c r="AO4" t="inlineStr"/>
       <c r="AP4" t="inlineStr"/>
       <c r="AQ4" t="n">
         <v>498991.2</v>
@@ -1862,9 +1784,7 @@
       <c r="AS4" t="n">
         <v>4.403333</v>
       </c>
-      <c r="AT4" t="n">
-        <v>38.7</v>
-      </c>
+      <c r="AT4" t="inlineStr"/>
       <c r="AU4" t="inlineStr"/>
       <c r="AV4" t="n">
         <v>26687.8</v>
@@ -1873,9 +1793,7 @@
       <c r="AX4" t="n">
         <v>15.32102</v>
       </c>
-      <c r="AY4" t="n">
-        <v>42.09999999999999</v>
-      </c>
+      <c r="AY4" t="inlineStr"/>
       <c r="AZ4" t="inlineStr"/>
       <c r="BA4" t="n">
         <v>8595.5</v>
@@ -1895,9 +1813,7 @@
       <c r="BH4" t="n">
         <v>7.133333</v>
       </c>
-      <c r="BI4" t="n">
-        <v>41.65000000000001</v>
-      </c>
+      <c r="BI4" t="inlineStr"/>
       <c r="BJ4" t="inlineStr"/>
       <c r="BK4" t="n">
         <v>13157.4</v>
@@ -1908,9 +1824,7 @@
       <c r="BM4" t="n">
         <v>6.153333</v>
       </c>
-      <c r="BN4" t="n">
-        <v>39.85</v>
-      </c>
+      <c r="BN4" t="inlineStr"/>
       <c r="BO4" t="inlineStr"/>
       <c r="BP4" t="n">
         <v>223373.8</v>
@@ -1921,9 +1835,7 @@
       <c r="BR4" t="n">
         <v>10.61</v>
       </c>
-      <c r="BS4" t="n">
-        <v>39.05</v>
-      </c>
+      <c r="BS4" t="inlineStr"/>
       <c r="BT4" t="inlineStr"/>
       <c r="BU4" t="n">
         <v>988.3</v>
@@ -1946,9 +1858,7 @@
         <v>7.030667</v>
       </c>
       <c r="CG4" t="inlineStr"/>
-      <c r="CH4" t="n">
-        <v>39.5</v>
-      </c>
+      <c r="CH4" t="inlineStr"/>
       <c r="CI4" t="inlineStr"/>
       <c r="CJ4" t="n">
         <v>85510.2</v>
@@ -1959,9 +1869,7 @@
       <c r="CL4" t="n">
         <v>4.066667</v>
       </c>
-      <c r="CM4" t="n">
-        <v>31.4</v>
-      </c>
+      <c r="CM4" t="inlineStr"/>
       <c r="CN4" t="inlineStr"/>
       <c r="CO4" t="n">
         <v>28780.8</v>
@@ -1972,9 +1880,7 @@
       <c r="CQ4" t="n">
         <v>5.44</v>
       </c>
-      <c r="CR4" t="n">
-        <v>34.65</v>
-      </c>
+      <c r="CR4" t="inlineStr"/>
       <c r="CS4" t="inlineStr"/>
       <c r="CT4" t="n">
         <v>27953.2</v>
@@ -1994,9 +1900,7 @@
       <c r="DA4" t="n">
         <v>9.337</v>
       </c>
-      <c r="DB4" t="n">
-        <v>41.2</v>
-      </c>
+      <c r="DB4" t="inlineStr"/>
       <c r="DC4" t="inlineStr"/>
       <c r="DD4" t="n">
         <v>8410.6</v>
@@ -2030,9 +1934,7 @@
       <c r="DU4" t="n">
         <v>9.543666999999999</v>
       </c>
-      <c r="DV4" t="n">
-        <v>38.15</v>
-      </c>
+      <c r="DV4" t="inlineStr"/>
       <c r="DW4" t="inlineStr"/>
       <c r="DX4" t="n">
         <v>47946.2</v>
@@ -2043,9 +1945,7 @@
       <c r="DZ4" t="n">
         <v>9.109999999999999</v>
       </c>
-      <c r="EA4" t="n">
-        <v>34.2</v>
-      </c>
+      <c r="EA4" t="inlineStr"/>
       <c r="EB4" t="inlineStr"/>
       <c r="EC4" t="n">
         <v>67566.8</v>
@@ -2065,9 +1965,7 @@
       <c r="EJ4" t="n">
         <v>6.84931</v>
       </c>
-      <c r="EK4" t="n">
-        <v>36.8</v>
-      </c>
+      <c r="EK4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -2085,9 +1983,7 @@
       <c r="E5" t="n">
         <v>4.176667</v>
       </c>
-      <c r="F5" t="n">
-        <v>39.84999999999999</v>
-      </c>
+      <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="n">
         <v>57115.3</v>
@@ -2098,9 +1994,7 @@
       <c r="J5" t="n">
         <v>3.96</v>
       </c>
-      <c r="K5" t="n">
-        <v>37.8</v>
-      </c>
+      <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr"/>
       <c r="M5" t="n">
         <v>4339.3</v>
@@ -2127,9 +2021,7 @@
       <c r="Y5" t="n">
         <v>5.350968</v>
       </c>
-      <c r="Z5" t="n">
-        <v>34.075</v>
-      </c>
+      <c r="Z5" t="inlineStr"/>
       <c r="AA5" t="inlineStr"/>
       <c r="AB5" t="n">
         <v>810.2</v>
@@ -2147,9 +2039,7 @@
       <c r="AI5" t="n">
         <v>5.026667</v>
       </c>
-      <c r="AJ5" t="n">
-        <v>37.425</v>
-      </c>
+      <c r="AJ5" t="inlineStr"/>
       <c r="AK5" t="inlineStr"/>
       <c r="AL5" t="n">
         <v>313056.6</v>
@@ -2160,9 +2050,7 @@
       <c r="AN5" t="n">
         <v>6.107234</v>
       </c>
-      <c r="AO5" t="n">
-        <v>39.625</v>
-      </c>
+      <c r="AO5" t="inlineStr"/>
       <c r="AP5" t="inlineStr"/>
       <c r="AQ5" t="n">
         <v>517170</v>
@@ -2173,9 +2061,7 @@
       <c r="AS5" t="n">
         <v>4.013333</v>
       </c>
-      <c r="AT5" t="n">
-        <v>38.7</v>
-      </c>
+      <c r="AT5" t="inlineStr"/>
       <c r="AU5" t="inlineStr"/>
       <c r="AV5" t="n">
         <v>27786.3</v>
@@ -2184,9 +2070,7 @@
       <c r="AX5" t="n">
         <v>15.71143</v>
       </c>
-      <c r="AY5" t="n">
-        <v>42</v>
-      </c>
+      <c r="AY5" t="inlineStr"/>
       <c r="AZ5" t="inlineStr"/>
       <c r="BA5" t="n">
         <v>9404.799999999999</v>
@@ -2206,9 +2090,7 @@
       <c r="BH5" t="n">
         <v>7.133333</v>
       </c>
-      <c r="BI5" t="n">
-        <v>41.875</v>
-      </c>
+      <c r="BI5" t="inlineStr"/>
       <c r="BJ5" t="inlineStr"/>
       <c r="BK5" t="n">
         <v>13490.6</v>
@@ -2219,9 +2101,7 @@
       <c r="BM5" t="n">
         <v>5.583333</v>
       </c>
-      <c r="BN5" t="n">
-        <v>39.975</v>
-      </c>
+      <c r="BN5" t="inlineStr"/>
       <c r="BO5" t="inlineStr"/>
       <c r="BP5" t="n">
         <v>251564.4</v>
@@ -2232,9 +2112,7 @@
       <c r="BR5" t="n">
         <v>10.68667</v>
       </c>
-      <c r="BS5" t="n">
-        <v>38.925</v>
-      </c>
+      <c r="BS5" t="inlineStr"/>
       <c r="BT5" t="inlineStr"/>
       <c r="BU5" t="n">
         <v>1064.8</v>
@@ -2257,9 +2135,7 @@
         <v>6.766667</v>
       </c>
       <c r="CG5" t="inlineStr"/>
-      <c r="CH5" t="n">
-        <v>39.4</v>
-      </c>
+      <c r="CH5" t="inlineStr"/>
       <c r="CI5" t="inlineStr"/>
       <c r="CJ5" t="n">
         <v>90770.10000000001</v>
@@ -2270,9 +2146,7 @@
       <c r="CL5" t="n">
         <v>3.806667</v>
       </c>
-      <c r="CM5" t="n">
-        <v>31.85</v>
-      </c>
+      <c r="CM5" t="inlineStr"/>
       <c r="CN5" t="inlineStr"/>
       <c r="CO5" t="n">
         <v>30592.3</v>
@@ -2283,9 +2157,7 @@
       <c r="CQ5" t="n">
         <v>5.33</v>
       </c>
-      <c r="CR5" t="n">
-        <v>34.775</v>
-      </c>
+      <c r="CR5" t="inlineStr"/>
       <c r="CS5" t="inlineStr"/>
       <c r="CT5" t="n">
         <v>28800.9</v>
@@ -2305,9 +2177,7 @@
       <c r="DA5" t="n">
         <v>9.082333999999999</v>
       </c>
-      <c r="DB5" t="n">
-        <v>41</v>
-      </c>
+      <c r="DB5" t="inlineStr"/>
       <c r="DC5" t="inlineStr"/>
       <c r="DD5" t="n">
         <v>7093.1</v>
@@ -2343,9 +2213,7 @@
       <c r="DU5" t="n">
         <v>9.390000000000001</v>
       </c>
-      <c r="DV5" t="n">
-        <v>38.075</v>
-      </c>
+      <c r="DV5" t="inlineStr"/>
       <c r="DW5" t="inlineStr"/>
       <c r="DX5" t="n">
         <v>58220.1</v>
@@ -2356,9 +2224,7 @@
       <c r="DZ5" t="n">
         <v>8.773334</v>
       </c>
-      <c r="EA5" t="n">
-        <v>34.3</v>
-      </c>
+      <c r="EA5" t="inlineStr"/>
       <c r="EB5" t="inlineStr"/>
       <c r="EC5" t="n">
         <v>70342</v>
@@ -2378,9 +2244,7 @@
       <c r="EJ5" t="n">
         <v>6.696187</v>
       </c>
-      <c r="EK5" t="n">
-        <v>36.75</v>
-      </c>
+      <c r="EK5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -2400,9 +2264,7 @@
       <c r="E6" t="n">
         <v>3.476667</v>
       </c>
-      <c r="F6" t="n">
-        <v>39.8</v>
-      </c>
+      <c r="F6" t="inlineStr"/>
       <c r="G6" t="n">
         <v>70.00333333333333</v>
       </c>
@@ -2415,9 +2277,7 @@
       <c r="J6" t="n">
         <v>3.35</v>
       </c>
-      <c r="K6" t="n">
-        <v>37.8</v>
-      </c>
+      <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr"/>
       <c r="M6" t="n">
         <v>3757.2</v>
@@ -2448,9 +2308,7 @@
       <c r="Y6" t="n">
         <v>4.451957</v>
       </c>
-      <c r="Z6" t="n">
-        <v>34</v>
-      </c>
+      <c r="Z6" t="inlineStr"/>
       <c r="AA6" t="n">
         <v>44.02</v>
       </c>
@@ -2474,9 +2332,7 @@
       <c r="AI6" t="n">
         <v>4.163333</v>
       </c>
-      <c r="AJ6" t="n">
-        <v>37.6</v>
-      </c>
+      <c r="AJ6" t="inlineStr"/>
       <c r="AK6" t="n">
         <v>74.48333333333333</v>
       </c>
@@ -2489,9 +2345,7 @@
       <c r="AN6" t="n">
         <v>4.460033</v>
       </c>
-      <c r="AO6" t="n">
-        <v>39.6</v>
-      </c>
+      <c r="AO6" t="inlineStr"/>
       <c r="AP6" t="n">
         <v>75.46666666666665</v>
       </c>
@@ -2504,9 +2358,7 @@
       <c r="AS6" t="n">
         <v>3.44</v>
       </c>
-      <c r="AT6" t="n">
-        <v>38.7</v>
-      </c>
+      <c r="AT6" t="inlineStr"/>
       <c r="AU6" t="n">
         <v>59.53333333333333</v>
       </c>
@@ -2517,9 +2369,7 @@
       <c r="AX6" t="n">
         <v>14.22553</v>
       </c>
-      <c r="AY6" t="n">
-        <v>41.9</v>
-      </c>
+      <c r="AY6" t="inlineStr"/>
       <c r="AZ6" t="n">
         <v>29.93333333333333</v>
       </c>
@@ -2530,9 +2380,7 @@
       <c r="BC6" t="n">
         <v>26.36667</v>
       </c>
-      <c r="BD6" t="n">
-        <v>41.2</v>
-      </c>
+      <c r="BD6" t="inlineStr"/>
       <c r="BE6" t="n">
         <v>42.83333333333334</v>
       </c>
@@ -2545,9 +2393,7 @@
       <c r="BH6" t="n">
         <v>7.566667</v>
       </c>
-      <c r="BI6" t="n">
-        <v>42.1</v>
-      </c>
+      <c r="BI6" t="inlineStr"/>
       <c r="BJ6" t="n">
         <v>68.53333333333333</v>
       </c>
@@ -2560,9 +2406,7 @@
       <c r="BM6" t="n">
         <v>5.106667</v>
       </c>
-      <c r="BN6" t="n">
-        <v>40.1</v>
-      </c>
+      <c r="BN6" t="inlineStr"/>
       <c r="BO6" t="n">
         <v>67.76666666666667</v>
       </c>
@@ -2575,9 +2419,7 @@
       <c r="BR6" t="n">
         <v>9.949999999999999</v>
       </c>
-      <c r="BS6" t="n">
-        <v>38.8</v>
-      </c>
+      <c r="BS6" t="inlineStr"/>
       <c r="BT6" t="n">
         <v>45.18666666666667</v>
       </c>
@@ -2606,9 +2448,7 @@
         <v>6.510667</v>
       </c>
       <c r="CG6" t="inlineStr"/>
-      <c r="CH6" t="n">
-        <v>39.3</v>
-      </c>
+      <c r="CH6" t="inlineStr"/>
       <c r="CI6" t="n">
         <v>68.44666666666667</v>
       </c>
@@ -2621,9 +2461,7 @@
       <c r="CL6" t="n">
         <v>3.183333</v>
       </c>
-      <c r="CM6" t="n">
-        <v>32.3</v>
-      </c>
+      <c r="CM6" t="inlineStr"/>
       <c r="CN6" t="n">
         <v>69.33333333333333</v>
       </c>
@@ -2636,9 +2474,7 @@
       <c r="CQ6" t="n">
         <v>5.22</v>
       </c>
-      <c r="CR6" t="n">
-        <v>34.9</v>
-      </c>
+      <c r="CR6" t="inlineStr"/>
       <c r="CS6" t="n">
         <v>43.63333333333333</v>
       </c>
@@ -2662,9 +2498,7 @@
       <c r="DA6" t="n">
         <v>8.166667</v>
       </c>
-      <c r="DB6" t="n">
-        <v>40.8</v>
-      </c>
+      <c r="DB6" t="inlineStr"/>
       <c r="DC6" t="n">
         <v>2.76</v>
       </c>
@@ -2695,9 +2529,7 @@
       </c>
       <c r="DO6" t="inlineStr"/>
       <c r="DP6" t="inlineStr"/>
-      <c r="DQ6" t="n">
-        <v>42.2</v>
-      </c>
+      <c r="DQ6" t="inlineStr"/>
       <c r="DR6" t="n">
         <v>64.12333333333333</v>
       </c>
@@ -2710,9 +2542,7 @@
       <c r="DU6" t="n">
         <v>8.68</v>
       </c>
-      <c r="DV6" t="n">
-        <v>38</v>
-      </c>
+      <c r="DV6" t="inlineStr"/>
       <c r="DW6" t="n">
         <v>75.71666666666665</v>
       </c>
@@ -2725,9 +2555,7 @@
       <c r="DZ6" t="n">
         <v>7.643333</v>
       </c>
-      <c r="EA6" t="n">
-        <v>34.4</v>
-      </c>
+      <c r="EA6" t="inlineStr"/>
       <c r="EB6" t="inlineStr"/>
       <c r="EC6" t="n">
         <v>67670.10000000001</v>
@@ -2736,9 +2564,7 @@
         <v>4.400333</v>
       </c>
       <c r="EE6" t="inlineStr"/>
-      <c r="EF6" t="n">
-        <v>37</v>
-      </c>
+      <c r="EF6" t="inlineStr"/>
       <c r="EG6" t="n">
         <v>68.10000000000001</v>
       </c>
@@ -2751,9 +2577,7 @@
       <c r="EJ6" t="n">
         <v>6.277534</v>
       </c>
-      <c r="EK6" t="n">
-        <v>36.7</v>
-      </c>
+      <c r="EK6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -2773,9 +2597,7 @@
       <c r="E7" t="n">
         <v>3.266667</v>
       </c>
-      <c r="F7" t="n">
-        <v>39.9</v>
-      </c>
+      <c r="F7" t="inlineStr"/>
       <c r="G7" t="n">
         <v>70.51666666666667</v>
       </c>
@@ -2788,9 +2610,7 @@
       <c r="J7" t="n">
         <v>3.243333</v>
       </c>
-      <c r="K7" t="n">
-        <v>37.825</v>
-      </c>
+      <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr"/>
       <c r="M7" t="n">
         <v>2561.8</v>
@@ -2821,9 +2641,7 @@
       <c r="Y7" t="n">
         <v>3.9251</v>
       </c>
-      <c r="Z7" t="n">
-        <v>34.1</v>
-      </c>
+      <c r="Z7" t="inlineStr"/>
       <c r="AA7" t="n">
         <v>45.96666666666667</v>
       </c>
@@ -2847,9 +2665,7 @@
       <c r="AI7" t="n">
         <v>3.766667</v>
       </c>
-      <c r="AJ7" t="n">
-        <v>38.05</v>
-      </c>
+      <c r="AJ7" t="inlineStr"/>
       <c r="AK7" t="n">
         <v>75.09666666666666</v>
       </c>
@@ -2862,9 +2678,7 @@
       <c r="AN7" t="n">
         <v>3.956633</v>
       </c>
-      <c r="AO7" t="n">
-        <v>39.5</v>
-      </c>
+      <c r="AO7" t="inlineStr"/>
       <c r="AP7" t="n">
         <v>75.7</v>
       </c>
@@ -2877,9 +2691,7 @@
       <c r="AS7" t="n">
         <v>3.336667</v>
       </c>
-      <c r="AT7" t="n">
-        <v>38.675</v>
-      </c>
+      <c r="AT7" t="inlineStr"/>
       <c r="AU7" t="n">
         <v>61.61666666666667</v>
       </c>
@@ -2890,9 +2702,7 @@
       <c r="AX7" t="n">
         <v>14.21426</v>
       </c>
-      <c r="AY7" t="n">
-        <v>41.875</v>
-      </c>
+      <c r="AY7" t="inlineStr"/>
       <c r="AZ7" t="n">
         <v>31.52</v>
       </c>
@@ -2903,9 +2713,7 @@
       <c r="BC7" t="n">
         <v>24.06667</v>
       </c>
-      <c r="BD7" t="n">
-        <v>41.40000000000001</v>
-      </c>
+      <c r="BD7" t="inlineStr"/>
       <c r="BE7" t="n">
         <v>43.21</v>
       </c>
@@ -2918,9 +2726,7 @@
       <c r="BH7" t="n">
         <v>6.566667</v>
       </c>
-      <c r="BI7" t="n">
-        <v>42.025</v>
-      </c>
+      <c r="BI7" t="inlineStr"/>
       <c r="BJ7" t="n">
         <v>68.93333333333334</v>
       </c>
@@ -2933,9 +2739,7 @@
       <c r="BM7" t="n">
         <v>5.11</v>
       </c>
-      <c r="BN7" t="n">
-        <v>39.95</v>
-      </c>
+      <c r="BN7" t="inlineStr"/>
       <c r="BO7" t="n">
         <v>68.5</v>
       </c>
@@ -2948,9 +2752,7 @@
       <c r="BR7" t="n">
         <v>9.103332999999999</v>
       </c>
-      <c r="BS7" t="n">
-        <v>38.9</v>
-      </c>
+      <c r="BS7" t="inlineStr"/>
       <c r="BT7" t="n">
         <v>46.51</v>
       </c>
@@ -2979,9 +2781,7 @@
         <v>6.520333</v>
       </c>
       <c r="CG7" t="inlineStr"/>
-      <c r="CH7" t="n">
-        <v>39.275</v>
-      </c>
+      <c r="CH7" t="inlineStr"/>
       <c r="CI7" t="n">
         <v>69.02</v>
       </c>
@@ -2994,9 +2794,7 @@
       <c r="CL7" t="n">
         <v>2.846667</v>
       </c>
-      <c r="CM7" t="n">
-        <v>32.3</v>
-      </c>
+      <c r="CM7" t="inlineStr"/>
       <c r="CN7" t="n">
         <v>69.86666666666667</v>
       </c>
@@ -3009,9 +2807,7 @@
       <c r="CQ7" t="n">
         <v>4.796667</v>
       </c>
-      <c r="CR7" t="n">
-        <v>35.1</v>
-      </c>
+      <c r="CR7" t="inlineStr"/>
       <c r="CS7" t="n">
         <v>45.73333333333333</v>
       </c>
@@ -3035,9 +2831,7 @@
       <c r="DA7" t="n">
         <v>7.333333</v>
       </c>
-      <c r="DB7" t="n">
-        <v>40.59999999999999</v>
-      </c>
+      <c r="DB7" t="inlineStr"/>
       <c r="DC7" t="n">
         <v>2.98</v>
       </c>
@@ -3068,9 +2862,7 @@
       </c>
       <c r="DO7" t="inlineStr"/>
       <c r="DP7" t="inlineStr"/>
-      <c r="DQ7" t="n">
-        <v>41.77500000000001</v>
-      </c>
+      <c r="DQ7" t="inlineStr"/>
       <c r="DR7" t="n">
         <v>64.88333333333334</v>
       </c>
@@ -3083,9 +2875,7 @@
       <c r="DU7" t="n">
         <v>7.45</v>
       </c>
-      <c r="DV7" t="n">
-        <v>38.075</v>
-      </c>
+      <c r="DV7" t="inlineStr"/>
       <c r="DW7" t="n">
         <v>76.44333333333333</v>
       </c>
@@ -3098,9 +2888,7 @@
       <c r="DZ7" t="n">
         <v>6.076667</v>
       </c>
-      <c r="EA7" t="n">
-        <v>34.875</v>
-      </c>
+      <c r="EA7" t="inlineStr"/>
       <c r="EB7" t="inlineStr"/>
       <c r="EC7" t="n">
         <v>67654.2</v>
@@ -3109,9 +2897,7 @@
         <v>4.546</v>
       </c>
       <c r="EE7" t="inlineStr"/>
-      <c r="EF7" t="n">
-        <v>37.025</v>
-      </c>
+      <c r="EF7" t="inlineStr"/>
       <c r="EG7" t="n">
         <v>68.86666666666667</v>
       </c>
@@ -3124,9 +2910,7 @@
       <c r="EJ7" t="n">
         <v>6.045267</v>
       </c>
-      <c r="EK7" t="n">
-        <v>36.65000000000001</v>
-      </c>
+      <c r="EK7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -3146,9 +2930,7 @@
       <c r="E8" t="n">
         <v>3.42</v>
       </c>
-      <c r="F8" t="n">
-        <v>40</v>
-      </c>
+      <c r="F8" t="inlineStr"/>
       <c r="G8" t="n">
         <v>70.44666666666667</v>
       </c>
@@ -3161,9 +2943,7 @@
       <c r="J8" t="n">
         <v>3.23</v>
       </c>
-      <c r="K8" t="n">
-        <v>37.84999999999999</v>
-      </c>
+      <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr"/>
       <c r="M8" t="n">
         <v>2300</v>
@@ -3194,9 +2974,7 @@
       <c r="Y8" t="n">
         <v>3.893764</v>
       </c>
-      <c r="Z8" t="n">
-        <v>34.2</v>
-      </c>
+      <c r="Z8" t="inlineStr"/>
       <c r="AA8" t="n">
         <v>46.13</v>
       </c>
@@ -3220,9 +2998,7 @@
       <c r="AI8" t="n">
         <v>3.483333</v>
       </c>
-      <c r="AJ8" t="n">
-        <v>38.5</v>
-      </c>
+      <c r="AJ8" t="inlineStr"/>
       <c r="AK8" t="n">
         <v>74.91333333333334</v>
       </c>
@@ -3235,9 +3011,7 @@
       <c r="AN8" t="n">
         <v>3.8498</v>
       </c>
-      <c r="AO8" t="n">
-        <v>39.40000000000001</v>
-      </c>
+      <c r="AO8" t="inlineStr"/>
       <c r="AP8" t="n">
         <v>75.93333333333334</v>
       </c>
@@ -3250,9 +3024,7 @@
       <c r="AS8" t="n">
         <v>3.263333</v>
       </c>
-      <c r="AT8" t="n">
-        <v>38.65000000000001</v>
-      </c>
+      <c r="AT8" t="inlineStr"/>
       <c r="AU8" t="n">
         <v>61.19</v>
       </c>
@@ -3263,9 +3035,7 @@
       <c r="AX8" t="n">
         <v>13.57264</v>
       </c>
-      <c r="AY8" t="n">
-        <v>41.84999999999999</v>
-      </c>
+      <c r="AY8" t="inlineStr"/>
       <c r="AZ8" t="n">
         <v>32.25</v>
       </c>
@@ -3276,9 +3046,7 @@
       <c r="BC8" t="n">
         <v>23.26667</v>
       </c>
-      <c r="BD8" t="n">
-        <v>41.6</v>
-      </c>
+      <c r="BD8" t="inlineStr"/>
       <c r="BE8" t="n">
         <v>43.42333333333332</v>
       </c>
@@ -3291,9 +3059,7 @@
       <c r="BH8" t="n">
         <v>6.733333</v>
       </c>
-      <c r="BI8" t="n">
-        <v>41.95</v>
-      </c>
+      <c r="BI8" t="inlineStr"/>
       <c r="BJ8" t="n">
         <v>69.3</v>
       </c>
@@ -3306,9 +3072,7 @@
       <c r="BM8" t="n">
         <v>5.7</v>
       </c>
-      <c r="BN8" t="n">
-        <v>39.8</v>
-      </c>
+      <c r="BN8" t="inlineStr"/>
       <c r="BO8" t="n">
         <v>68.66666666666667</v>
       </c>
@@ -3321,9 +3085,7 @@
       <c r="BR8" t="n">
         <v>8.666667</v>
       </c>
-      <c r="BS8" t="n">
-        <v>39</v>
-      </c>
+      <c r="BS8" t="inlineStr"/>
       <c r="BT8" t="n">
         <v>47.08000000000001</v>
       </c>
@@ -3352,9 +3114,7 @@
         <v>6.377333</v>
       </c>
       <c r="CG8" t="inlineStr"/>
-      <c r="CH8" t="n">
-        <v>39.25</v>
-      </c>
+      <c r="CH8" t="inlineStr"/>
       <c r="CI8" t="n">
         <v>68.65333333333332</v>
       </c>
@@ -3367,9 +3127,7 @@
       <c r="CL8" t="n">
         <v>2.966667</v>
       </c>
-      <c r="CM8" t="n">
-        <v>32.3</v>
-      </c>
+      <c r="CM8" t="inlineStr"/>
       <c r="CN8" t="n">
         <v>70.23333333333333</v>
       </c>
@@ -3382,9 +3140,7 @@
       <c r="CQ8" t="n">
         <v>5.033333</v>
       </c>
-      <c r="CR8" t="n">
-        <v>35.3</v>
-      </c>
+      <c r="CR8" t="inlineStr"/>
       <c r="CS8" t="n">
         <v>46.7</v>
       </c>
@@ -3408,9 +3164,7 @@
       <c r="DA8" t="n">
         <v>7.233333</v>
       </c>
-      <c r="DB8" t="n">
-        <v>40.4</v>
-      </c>
+      <c r="DB8" t="inlineStr"/>
       <c r="DC8" t="n">
         <v>3.39</v>
       </c>
@@ -3441,9 +3195,7 @@
       </c>
       <c r="DO8" t="inlineStr"/>
       <c r="DP8" t="inlineStr"/>
-      <c r="DQ8" t="n">
-        <v>41.35</v>
-      </c>
+      <c r="DQ8" t="inlineStr"/>
       <c r="DR8" t="n">
         <v>65.18666666666667</v>
       </c>
@@ -3456,9 +3208,7 @@
       <c r="DU8" t="n">
         <v>7.213333</v>
       </c>
-      <c r="DV8" t="n">
-        <v>38.15</v>
-      </c>
+      <c r="DV8" t="inlineStr"/>
       <c r="DW8" t="n">
         <v>76.13666666666667</v>
       </c>
@@ -3471,9 +3221,7 @@
       <c r="DZ8" t="n">
         <v>5.133333</v>
       </c>
-      <c r="EA8" t="n">
-        <v>35.34999999999999</v>
-      </c>
+      <c r="EA8" t="inlineStr"/>
       <c r="EB8" t="inlineStr"/>
       <c r="EC8" t="n">
         <v>67027.2</v>
@@ -3482,9 +3230,7 @@
         <v>4.428</v>
       </c>
       <c r="EE8" t="inlineStr"/>
-      <c r="EF8" t="n">
-        <v>37.05</v>
-      </c>
+      <c r="EF8" t="inlineStr"/>
       <c r="EG8" t="n">
         <v>68.93333333333334</v>
       </c>
@@ -3497,9 +3243,7 @@
       <c r="EJ8" t="n">
         <v>5.840597</v>
       </c>
-      <c r="EK8" t="n">
-        <v>36.6</v>
-      </c>
+      <c r="EK8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -3519,9 +3263,7 @@
       <c r="E9" t="n">
         <v>3.33</v>
       </c>
-      <c r="F9" t="n">
-        <v>40.1</v>
-      </c>
+      <c r="F9" t="inlineStr"/>
       <c r="G9" t="n">
         <v>70.93666666666667</v>
       </c>
@@ -3534,9 +3276,7 @@
       <c r="J9" t="n">
         <v>3.043333</v>
       </c>
-      <c r="K9" t="n">
-        <v>37.875</v>
-      </c>
+      <c r="K9" t="inlineStr"/>
       <c r="L9" t="n">
         <v>7.28</v>
       </c>
@@ -3569,9 +3309,7 @@
       <c r="Y9" t="n">
         <v>3.662975</v>
       </c>
-      <c r="Z9" t="n">
-        <v>34.3</v>
-      </c>
+      <c r="Z9" t="inlineStr"/>
       <c r="AA9" t="n">
         <v>46.66999999999999</v>
       </c>
@@ -3595,9 +3333,7 @@
       <c r="AI9" t="n">
         <v>3.086667</v>
       </c>
-      <c r="AJ9" t="n">
-        <v>38.95</v>
-      </c>
+      <c r="AJ9" t="inlineStr"/>
       <c r="AK9" t="n">
         <v>75.23666666666666</v>
       </c>
@@ -3610,9 +3346,7 @@
       <c r="AN9" t="n">
         <v>3.476033</v>
       </c>
-      <c r="AO9" t="n">
-        <v>39.3</v>
-      </c>
+      <c r="AO9" t="inlineStr"/>
       <c r="AP9" t="n">
         <v>75.83333333333333</v>
       </c>
@@ -3625,9 +3359,7 @@
       <c r="AS9" t="n">
         <v>3.18</v>
       </c>
-      <c r="AT9" t="n">
-        <v>38.625</v>
-      </c>
+      <c r="AT9" t="inlineStr"/>
       <c r="AU9" t="n">
         <v>62.88666666666666</v>
       </c>
@@ -3638,9 +3370,7 @@
       <c r="AX9" t="n">
         <v>13.11385</v>
       </c>
-      <c r="AY9" t="n">
-        <v>41.825</v>
-      </c>
+      <c r="AY9" t="inlineStr"/>
       <c r="AZ9" t="n">
         <v>33.32</v>
       </c>
@@ -3651,9 +3381,7 @@
       <c r="BC9" t="n">
         <v>22.13333</v>
       </c>
-      <c r="BD9" t="n">
-        <v>41.8</v>
-      </c>
+      <c r="BD9" t="inlineStr"/>
       <c r="BE9" t="n">
         <v>43.56666666666666</v>
       </c>
@@ -3666,9 +3394,7 @@
       <c r="BH9" t="n">
         <v>7.1</v>
       </c>
-      <c r="BI9" t="n">
-        <v>41.875</v>
-      </c>
+      <c r="BI9" t="inlineStr"/>
       <c r="BJ9" t="n">
         <v>69.76666666666667</v>
       </c>
@@ -3681,9 +3407,7 @@
       <c r="BM9" t="n">
         <v>5.756667</v>
       </c>
-      <c r="BN9" t="n">
-        <v>39.65</v>
-      </c>
+      <c r="BN9" t="inlineStr"/>
       <c r="BO9" t="n">
         <v>69.03333333333333</v>
       </c>
@@ -3696,9 +3420,7 @@
       <c r="BR9" t="n">
         <v>7.56</v>
       </c>
-      <c r="BS9" t="n">
-        <v>39.1</v>
-      </c>
+      <c r="BS9" t="inlineStr"/>
       <c r="BT9" t="n">
         <v>48.08333333333334</v>
       </c>
@@ -3727,9 +3449,7 @@
         <v>5.874667</v>
       </c>
       <c r="CG9" t="inlineStr"/>
-      <c r="CH9" t="n">
-        <v>39.225</v>
-      </c>
+      <c r="CH9" t="inlineStr"/>
       <c r="CI9" t="n">
         <v>69.20333333333333</v>
       </c>
@@ -3742,9 +3462,7 @@
       <c r="CL9" t="n">
         <v>2.993333</v>
       </c>
-      <c r="CM9" t="n">
-        <v>32.3</v>
-      </c>
+      <c r="CM9" t="inlineStr"/>
       <c r="CN9" t="n">
         <v>70.7</v>
       </c>
@@ -3757,9 +3475,7 @@
       <c r="CQ9" t="n">
         <v>4.523334</v>
       </c>
-      <c r="CR9" t="n">
-        <v>35.5</v>
-      </c>
+      <c r="CR9" t="inlineStr"/>
       <c r="CS9" t="n">
         <v>48.70000000000001</v>
       </c>
@@ -3783,9 +3499,7 @@
       <c r="DA9" t="n">
         <v>6.733333</v>
       </c>
-      <c r="DB9" t="n">
-        <v>40.2</v>
-      </c>
+      <c r="DB9" t="inlineStr"/>
       <c r="DC9" t="n">
         <v>3.873333333333334</v>
       </c>
@@ -3816,9 +3530,7 @@
       </c>
       <c r="DO9" t="inlineStr"/>
       <c r="DP9" t="inlineStr"/>
-      <c r="DQ9" t="n">
-        <v>40.925</v>
-      </c>
+      <c r="DQ9" t="inlineStr"/>
       <c r="DR9" t="n">
         <v>65.51333333333334</v>
       </c>
@@ -3831,9 +3543,7 @@
       <c r="DU9" t="n">
         <v>6.636667</v>
       </c>
-      <c r="DV9" t="n">
-        <v>38.22499999999999</v>
-      </c>
+      <c r="DV9" t="inlineStr"/>
       <c r="DW9" t="n">
         <v>76.33666666666666</v>
       </c>
@@ -3846,9 +3556,7 @@
       <c r="DZ9" t="n">
         <v>4.306667</v>
       </c>
-      <c r="EA9" t="n">
-        <v>35.825</v>
-      </c>
+      <c r="EA9" t="inlineStr"/>
       <c r="EB9" t="inlineStr"/>
       <c r="EC9" t="n">
         <v>65833.5</v>
@@ -3857,9 +3565,7 @@
         <v>4.160666</v>
       </c>
       <c r="EE9" t="inlineStr"/>
-      <c r="EF9" t="n">
-        <v>37.075</v>
-      </c>
+      <c r="EF9" t="inlineStr"/>
       <c r="EG9" t="n">
         <v>69.36666666666666</v>
       </c>
@@ -3872,9 +3578,7 @@
       <c r="EJ9" t="n">
         <v>6.278986</v>
       </c>
-      <c r="EK9" t="n">
-        <v>36.55</v>
-      </c>
+      <c r="EK9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -3894,9 +3598,7 @@
       <c r="E10" t="n">
         <v>3.323333</v>
       </c>
-      <c r="F10" t="n">
-        <v>40.2</v>
-      </c>
+      <c r="F10" t="inlineStr"/>
       <c r="G10" t="n">
         <v>71.24666666666667</v>
       </c>
@@ -3909,9 +3611,7 @@
       <c r="J10" t="n">
         <v>3.203333</v>
       </c>
-      <c r="K10" t="n">
-        <v>37.9</v>
-      </c>
+      <c r="K10" t="inlineStr"/>
       <c r="L10" t="n">
         <v>29.32</v>
       </c>
@@ -3931,9 +3631,7 @@
       <c r="T10" t="n">
         <v>12.38347</v>
       </c>
-      <c r="U10" t="n">
-        <v>43.4</v>
-      </c>
+      <c r="U10" t="inlineStr"/>
       <c r="V10" t="n">
         <v>72.33333333333333</v>
       </c>
@@ -3946,9 +3644,7 @@
       <c r="Y10" t="n">
         <v>3.647101</v>
       </c>
-      <c r="Z10" t="n">
-        <v>34.4</v>
-      </c>
+      <c r="Z10" t="inlineStr"/>
       <c r="AA10" t="n">
         <v>47.87</v>
       </c>
@@ -3959,9 +3655,7 @@
       <c r="AD10" t="n">
         <v>7.98</v>
       </c>
-      <c r="AE10" t="n">
-        <v>41.3</v>
-      </c>
+      <c r="AE10" t="inlineStr"/>
       <c r="AF10" t="n">
         <v>71.96666666666665</v>
       </c>
@@ -3974,9 +3668,7 @@
       <c r="AI10" t="n">
         <v>3.07</v>
       </c>
-      <c r="AJ10" t="n">
-        <v>39.4</v>
-      </c>
+      <c r="AJ10" t="inlineStr"/>
       <c r="AK10" t="n">
         <v>75.63333333333333</v>
       </c>
@@ -3989,9 +3681,7 @@
       <c r="AN10" t="n">
         <v>3.349367</v>
       </c>
-      <c r="AO10" t="n">
-        <v>39.2</v>
-      </c>
+      <c r="AO10" t="inlineStr"/>
       <c r="AP10" t="n">
         <v>76.66666666666667</v>
       </c>
@@ -4004,9 +3694,7 @@
       <c r="AS10" t="n">
         <v>3.196667</v>
       </c>
-      <c r="AT10" t="n">
-        <v>38.6</v>
-      </c>
+      <c r="AT10" t="inlineStr"/>
       <c r="AU10" t="n">
         <v>63.29333333333333</v>
       </c>
@@ -4017,9 +3705,7 @@
       <c r="AX10" t="n">
         <v>11.87371</v>
       </c>
-      <c r="AY10" t="n">
-        <v>41.8</v>
-      </c>
+      <c r="AY10" t="inlineStr"/>
       <c r="AZ10" t="n">
         <v>35.61666666666667</v>
       </c>
@@ -4030,9 +3716,7 @@
       <c r="BC10" t="n">
         <v>21.13333</v>
       </c>
-      <c r="BD10" t="n">
-        <v>42</v>
-      </c>
+      <c r="BD10" t="inlineStr"/>
       <c r="BE10" t="n">
         <v>43.64333333333334</v>
       </c>
@@ -4045,9 +3729,7 @@
       <c r="BH10" t="n">
         <v>7.133333</v>
       </c>
-      <c r="BI10" t="n">
-        <v>41.8</v>
-      </c>
+      <c r="BI10" t="inlineStr"/>
       <c r="BJ10" t="n">
         <v>69.63333333333333</v>
       </c>
@@ -4060,9 +3742,7 @@
       <c r="BM10" t="n">
         <v>5.776667</v>
       </c>
-      <c r="BN10" t="n">
-        <v>39.5</v>
-      </c>
+      <c r="BN10" t="inlineStr"/>
       <c r="BO10" t="n">
         <v>69.39999999999999</v>
       </c>
@@ -4075,9 +3755,7 @@
       <c r="BR10" t="n">
         <v>7.34</v>
       </c>
-      <c r="BS10" t="n">
-        <v>39.2</v>
-      </c>
+      <c r="BS10" t="inlineStr"/>
       <c r="BT10" t="n">
         <v>49.62333333333333</v>
       </c>
@@ -4106,9 +3784,7 @@
         <v>5.585</v>
       </c>
       <c r="CG10" t="inlineStr"/>
-      <c r="CH10" t="n">
-        <v>39.2</v>
-      </c>
+      <c r="CH10" t="inlineStr"/>
       <c r="CI10" t="n">
         <v>69.43333333333334</v>
       </c>
@@ -4121,9 +3797,7 @@
       <c r="CL10" t="n">
         <v>3.08</v>
       </c>
-      <c r="CM10" t="n">
-        <v>32.3</v>
-      </c>
+      <c r="CM10" t="inlineStr"/>
       <c r="CN10" t="n">
         <v>71.60000000000001</v>
       </c>
@@ -4136,9 +3810,7 @@
       <c r="CQ10" t="n">
         <v>3.516667</v>
       </c>
-      <c r="CR10" t="n">
-        <v>35.7</v>
-      </c>
+      <c r="CR10" t="inlineStr"/>
       <c r="CS10" t="n">
         <v>51.13333333333333</v>
       </c>
@@ -4149,9 +3821,7 @@
       <c r="CV10" t="n">
         <v>21.77333</v>
       </c>
-      <c r="CW10" t="n">
-        <v>42.2</v>
-      </c>
+      <c r="CW10" t="inlineStr"/>
       <c r="CX10" t="n">
         <v>67.7</v>
       </c>
@@ -4164,9 +3834,7 @@
       <c r="DA10" t="n">
         <v>6.233333</v>
       </c>
-      <c r="DB10" t="n">
-        <v>40</v>
-      </c>
+      <c r="DB10" t="inlineStr"/>
       <c r="DC10" t="n">
         <v>5.963333333333334</v>
       </c>
@@ -4177,9 +3845,7 @@
       <c r="DF10" t="n">
         <v>121.34</v>
       </c>
-      <c r="DG10" t="n">
-        <v>40.3</v>
-      </c>
+      <c r="DG10" t="inlineStr"/>
       <c r="DH10" t="n">
         <v>45.71</v>
       </c>
@@ -4199,9 +3865,7 @@
       </c>
       <c r="DO10" t="inlineStr"/>
       <c r="DP10" t="inlineStr"/>
-      <c r="DQ10" t="n">
-        <v>40.5</v>
-      </c>
+      <c r="DQ10" t="inlineStr"/>
       <c r="DR10" t="n">
         <v>65.75</v>
       </c>
@@ -4214,9 +3878,7 @@
       <c r="DU10" t="n">
         <v>5.883333</v>
       </c>
-      <c r="DV10" t="n">
-        <v>38.3</v>
-      </c>
+      <c r="DV10" t="inlineStr"/>
       <c r="DW10" t="n">
         <v>76.59333333333335</v>
       </c>
@@ -4229,9 +3891,7 @@
       <c r="DZ10" t="n">
         <v>3.94</v>
       </c>
-      <c r="EA10" t="n">
-        <v>36.3</v>
-      </c>
+      <c r="EA10" t="inlineStr"/>
       <c r="EB10" t="inlineStr"/>
       <c r="EC10" t="n">
         <v>61471.8</v>
@@ -4240,9 +3900,7 @@
         <v>3.776333</v>
       </c>
       <c r="EE10" t="inlineStr"/>
-      <c r="EF10" t="n">
-        <v>37.1</v>
-      </c>
+      <c r="EF10" t="inlineStr"/>
       <c r="EG10" t="n">
         <v>69.36666666666667</v>
       </c>
@@ -4255,9 +3913,7 @@
       <c r="EJ10" t="n">
         <v>6.33584</v>
       </c>
-      <c r="EK10" t="n">
-        <v>36.5</v>
-      </c>
+      <c r="EK10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -4277,9 +3933,7 @@
       <c r="E11" t="n">
         <v>3.416667</v>
       </c>
-      <c r="F11" t="n">
-        <v>40.1</v>
-      </c>
+      <c r="F11" t="inlineStr"/>
       <c r="G11" t="n">
         <v>71.48333333333333</v>
       </c>
@@ -4292,9 +3946,7 @@
       <c r="J11" t="n">
         <v>3.256667</v>
       </c>
-      <c r="K11" t="n">
-        <v>37.9</v>
-      </c>
+      <c r="K11" t="inlineStr"/>
       <c r="L11" t="n">
         <v>40.53333333333334</v>
       </c>
@@ -4314,9 +3966,7 @@
       <c r="T11" t="n">
         <v>19.67038</v>
       </c>
-      <c r="U11" t="n">
-        <v>43.325</v>
-      </c>
+      <c r="U11" t="inlineStr"/>
       <c r="V11" t="n">
         <v>73.06666666666666</v>
       </c>
@@ -4329,9 +3979,7 @@
       <c r="Y11" t="n">
         <v>3.641817</v>
       </c>
-      <c r="Z11" t="n">
-        <v>34.4</v>
-      </c>
+      <c r="Z11" t="inlineStr"/>
       <c r="AA11" t="n">
         <v>49.63666666666666</v>
       </c>
@@ -4342,9 +3990,7 @@
       <c r="AD11" t="n">
         <v>7.356667</v>
       </c>
-      <c r="AE11" t="n">
-        <v>41.3</v>
-      </c>
+      <c r="AE11" t="inlineStr"/>
       <c r="AF11" t="n">
         <v>72.61333333333333</v>
       </c>
@@ -4357,9 +4003,7 @@
       <c r="AI11" t="n">
         <v>3.076667</v>
       </c>
-      <c r="AJ11" t="n">
-        <v>39.175</v>
-      </c>
+      <c r="AJ11" t="inlineStr"/>
       <c r="AK11" t="n">
         <v>75.81999999999999</v>
       </c>
@@ -4372,9 +4016,7 @@
       <c r="AN11" t="n">
         <v>3.436567</v>
       </c>
-      <c r="AO11" t="n">
-        <v>39.225</v>
-      </c>
+      <c r="AO11" t="inlineStr"/>
       <c r="AP11" t="n">
         <v>76.73333333333333</v>
       </c>
@@ -4387,9 +4029,7 @@
       <c r="AS11" t="n">
         <v>3.18</v>
       </c>
-      <c r="AT11" t="n">
-        <v>38.6</v>
-      </c>
+      <c r="AT11" t="inlineStr"/>
       <c r="AU11" t="n">
         <v>65.02999999999999</v>
       </c>
@@ -4400,9 +4040,7 @@
       <c r="AX11" t="n">
         <v>10.91704</v>
       </c>
-      <c r="AY11" t="n">
-        <v>41.45</v>
-      </c>
+      <c r="AY11" t="inlineStr"/>
       <c r="AZ11" t="n">
         <v>37.33333333333334</v>
       </c>
@@ -4413,9 +4051,7 @@
       <c r="BC11" t="n">
         <v>20.63333</v>
       </c>
-      <c r="BD11" t="n">
-        <v>42</v>
-      </c>
+      <c r="BD11" t="inlineStr"/>
       <c r="BE11" t="n">
         <v>43.97666666666667</v>
       </c>
@@ -4428,9 +4064,7 @@
       <c r="BH11" t="n">
         <v>7.033333</v>
       </c>
-      <c r="BI11" t="n">
-        <v>41.8</v>
-      </c>
+      <c r="BI11" t="inlineStr"/>
       <c r="BJ11" t="n">
         <v>69.96666666666667</v>
       </c>
@@ -4443,9 +4077,7 @@
       <c r="BM11" t="n">
         <v>6.233333</v>
       </c>
-      <c r="BN11" t="n">
-        <v>39.5</v>
-      </c>
+      <c r="BN11" t="inlineStr"/>
       <c r="BO11" t="n">
         <v>69.73333333333333</v>
       </c>
@@ -4458,9 +4090,7 @@
       <c r="BR11" t="n">
         <v>6.946667</v>
       </c>
-      <c r="BS11" t="n">
-        <v>39.175</v>
-      </c>
+      <c r="BS11" t="inlineStr"/>
       <c r="BT11" t="n">
         <v>50.38333333333333</v>
       </c>
@@ -4489,9 +4119,7 @@
         <v>5.661667</v>
       </c>
       <c r="CG11" t="inlineStr"/>
-      <c r="CH11" t="n">
-        <v>39.2</v>
-      </c>
+      <c r="CH11" t="inlineStr"/>
       <c r="CI11" t="n">
         <v>69.96333333333334</v>
       </c>
@@ -4504,9 +4132,7 @@
       <c r="CL11" t="n">
         <v>3.216667</v>
       </c>
-      <c r="CM11" t="n">
-        <v>32.3</v>
-      </c>
+      <c r="CM11" t="inlineStr"/>
       <c r="CN11" t="n">
         <v>71.8</v>
       </c>
@@ -4519,9 +4145,7 @@
       <c r="CQ11" t="n">
         <v>3.49</v>
       </c>
-      <c r="CR11" t="n">
-        <v>35.7</v>
-      </c>
+      <c r="CR11" t="inlineStr"/>
       <c r="CS11" t="n">
         <v>52.6</v>
       </c>
@@ -4532,9 +4156,7 @@
       <c r="CV11" t="n">
         <v>22.13</v>
       </c>
-      <c r="CW11" t="n">
-        <v>42.2</v>
-      </c>
+      <c r="CW11" t="inlineStr"/>
       <c r="CX11" t="n">
         <v>68.07666666666667</v>
       </c>
@@ -4547,9 +4169,7 @@
       <c r="DA11" t="n">
         <v>5.866667</v>
       </c>
-      <c r="DB11" t="n">
-        <v>40.2</v>
-      </c>
+      <c r="DB11" t="inlineStr"/>
       <c r="DC11" t="n">
         <v>8.23</v>
       </c>
@@ -4560,9 +4180,7 @@
       <c r="DF11" t="n">
         <v>118.7667</v>
       </c>
-      <c r="DG11" t="n">
-        <v>40.3</v>
-      </c>
+      <c r="DG11" t="inlineStr"/>
       <c r="DH11" t="n">
         <v>46.18333333333334</v>
       </c>
@@ -4580,9 +4198,7 @@
       </c>
       <c r="DO11" t="inlineStr"/>
       <c r="DP11" t="inlineStr"/>
-      <c r="DQ11" t="n">
-        <v>40.5</v>
-      </c>
+      <c r="DQ11" t="inlineStr"/>
       <c r="DR11" t="n">
         <v>65.81666666666666</v>
       </c>
@@ -4595,9 +4211,7 @@
       <c r="DU11" t="n">
         <v>5.35</v>
       </c>
-      <c r="DV11" t="n">
-        <v>38.375</v>
-      </c>
+      <c r="DV11" t="inlineStr"/>
       <c r="DW11" t="n">
         <v>77.44666666666667</v>
       </c>
@@ -4610,9 +4224,7 @@
       <c r="DZ11" t="n">
         <v>4.056667</v>
       </c>
-      <c r="EA11" t="n">
-        <v>36.3</v>
-      </c>
+      <c r="EA11" t="inlineStr"/>
       <c r="EB11" t="inlineStr"/>
       <c r="EC11" t="n">
         <v>64510.2</v>
@@ -4621,9 +4233,7 @@
         <v>3.625667</v>
       </c>
       <c r="EE11" t="inlineStr"/>
-      <c r="EF11" t="n">
-        <v>37.1</v>
-      </c>
+      <c r="EF11" t="inlineStr"/>
       <c r="EG11" t="n">
         <v>70</v>
       </c>
@@ -4636,9 +4246,7 @@
       <c r="EJ11" t="n">
         <v>6.550377</v>
       </c>
-      <c r="EK11" t="n">
-        <v>36.5</v>
-      </c>
+      <c r="EK11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -4658,9 +4266,7 @@
       <c r="E12" t="n">
         <v>3.443333</v>
       </c>
-      <c r="F12" t="n">
-        <v>40</v>
-      </c>
+      <c r="F12" t="inlineStr"/>
       <c r="G12" t="n">
         <v>71.67</v>
       </c>
@@ -4673,9 +4279,7 @@
       <c r="J12" t="n">
         <v>3.543333</v>
       </c>
-      <c r="K12" t="n">
-        <v>37.9</v>
-      </c>
+      <c r="K12" t="inlineStr"/>
       <c r="L12" t="n">
         <v>44.30666666666666</v>
       </c>
@@ -4695,9 +4299,7 @@
       <c r="T12" t="n">
         <v>15.47684</v>
       </c>
-      <c r="U12" t="n">
-        <v>43.25</v>
-      </c>
+      <c r="U12" t="inlineStr"/>
       <c r="V12" t="n">
         <v>73.10000000000001</v>
       </c>
@@ -4710,9 +4312,7 @@
       <c r="Y12" t="n">
         <v>3.646961</v>
       </c>
-      <c r="Z12" t="n">
-        <v>34.4</v>
-      </c>
+      <c r="Z12" t="inlineStr"/>
       <c r="AA12" t="n">
         <v>50.6</v>
       </c>
@@ -4723,9 +4323,7 @@
       <c r="AD12" t="n">
         <v>6.976666</v>
       </c>
-      <c r="AE12" t="n">
-        <v>41.3</v>
-      </c>
+      <c r="AE12" t="inlineStr"/>
       <c r="AF12" t="n">
         <v>72.89999999999999</v>
       </c>
@@ -4738,9 +4336,7 @@
       <c r="AI12" t="n">
         <v>3.173333</v>
       </c>
-      <c r="AJ12" t="n">
-        <v>38.95</v>
-      </c>
+      <c r="AJ12" t="inlineStr"/>
       <c r="AK12" t="n">
         <v>75.93333333333332</v>
       </c>
@@ -4753,9 +4349,7 @@
       <c r="AN12" t="n">
         <v>3.4093</v>
       </c>
-      <c r="AO12" t="n">
-        <v>39.25</v>
-      </c>
+      <c r="AO12" t="inlineStr"/>
       <c r="AP12" t="n">
         <v>77.13333333333334</v>
       </c>
@@ -4768,9 +4362,7 @@
       <c r="AS12" t="n">
         <v>3.236667</v>
       </c>
-      <c r="AT12" t="n">
-        <v>38.6</v>
-      </c>
+      <c r="AT12" t="inlineStr"/>
       <c r="AU12" t="n">
         <v>64.39666666666666</v>
       </c>
@@ -4783,9 +4375,7 @@
       <c r="AX12" t="n">
         <v>11.35479</v>
       </c>
-      <c r="AY12" t="n">
-        <v>41.09999999999999</v>
-      </c>
+      <c r="AY12" t="inlineStr"/>
       <c r="AZ12" t="n">
         <v>38.10666666666667</v>
       </c>
@@ -4796,9 +4386,7 @@
       <c r="BC12" t="n">
         <v>19.53333</v>
       </c>
-      <c r="BD12" t="n">
-        <v>42</v>
-      </c>
+      <c r="BD12" t="inlineStr"/>
       <c r="BE12" t="n">
         <v>44.14666666666667</v>
       </c>
@@ -4811,9 +4399,7 @@
       <c r="BH12" t="n">
         <v>6.966667</v>
       </c>
-      <c r="BI12" t="n">
-        <v>41.8</v>
-      </c>
+      <c r="BI12" t="inlineStr"/>
       <c r="BJ12" t="n">
         <v>69.96666666666665</v>
       </c>
@@ -4826,9 +4412,7 @@
       <c r="BM12" t="n">
         <v>6.22</v>
       </c>
-      <c r="BN12" t="n">
-        <v>39.5</v>
-      </c>
+      <c r="BN12" t="inlineStr"/>
       <c r="BO12" t="n">
         <v>69.8</v>
       </c>
@@ -4841,9 +4425,7 @@
       <c r="BR12" t="n">
         <v>6.81</v>
       </c>
-      <c r="BS12" t="n">
-        <v>39.15000000000001</v>
-      </c>
+      <c r="BS12" t="inlineStr"/>
       <c r="BT12" t="n">
         <v>50.58333333333334</v>
       </c>
@@ -4872,9 +4454,7 @@
         <v>5.596334</v>
       </c>
       <c r="CG12" t="inlineStr"/>
-      <c r="CH12" t="n">
-        <v>39.2</v>
-      </c>
+      <c r="CH12" t="inlineStr"/>
       <c r="CI12" t="n">
         <v>70.23666666666666</v>
       </c>
@@ -4887,9 +4467,7 @@
       <c r="CL12" t="n">
         <v>3.366667</v>
       </c>
-      <c r="CM12" t="n">
-        <v>32.3</v>
-      </c>
+      <c r="CM12" t="inlineStr"/>
       <c r="CN12" t="n">
         <v>71.66666666666667</v>
       </c>
@@ -4902,9 +4480,7 @@
       <c r="CQ12" t="n">
         <v>3.993333</v>
       </c>
-      <c r="CR12" t="n">
-        <v>35.7</v>
-      </c>
+      <c r="CR12" t="inlineStr"/>
       <c r="CS12" t="n">
         <v>53.56666666666666</v>
       </c>
@@ -4915,9 +4491,7 @@
       <c r="CV12" t="n">
         <v>24.22667</v>
       </c>
-      <c r="CW12" t="n">
-        <v>42.2</v>
-      </c>
+      <c r="CW12" t="inlineStr"/>
       <c r="CX12" t="n">
         <v>68.30333333333333</v>
       </c>
@@ -4930,9 +4504,7 @@
       <c r="DA12" t="n">
         <v>5.566667</v>
       </c>
-      <c r="DB12" t="n">
-        <v>40.4</v>
-      </c>
+      <c r="DB12" t="inlineStr"/>
       <c r="DC12" t="n">
         <v>8.82</v>
       </c>
@@ -4943,9 +4515,7 @@
       <c r="DF12" t="n">
         <v>49.49</v>
       </c>
-      <c r="DG12" t="n">
-        <v>40.3</v>
-      </c>
+      <c r="DG12" t="inlineStr"/>
       <c r="DH12" t="n">
         <v>46.66333333333333</v>
       </c>
@@ -4963,9 +4533,7 @@
       </c>
       <c r="DO12" t="inlineStr"/>
       <c r="DP12" t="inlineStr"/>
-      <c r="DQ12" t="n">
-        <v>40.5</v>
-      </c>
+      <c r="DQ12" t="inlineStr"/>
       <c r="DR12" t="n">
         <v>66.29333333333334</v>
       </c>
@@ -4978,9 +4546,7 @@
       <c r="DU12" t="n">
         <v>5.26</v>
       </c>
-      <c r="DV12" t="n">
-        <v>38.45</v>
-      </c>
+      <c r="DV12" t="inlineStr"/>
       <c r="DW12" t="n">
         <v>77.73666666666666</v>
       </c>
@@ -4993,9 +4559,7 @@
       <c r="DZ12" t="n">
         <v>4.113333</v>
       </c>
-      <c r="EA12" t="n">
-        <v>36.3</v>
-      </c>
+      <c r="EA12" t="inlineStr"/>
       <c r="EB12" t="inlineStr"/>
       <c r="EC12" t="n">
         <v>65894.89999999999</v>
@@ -5004,9 +4568,7 @@
         <v>3.660333</v>
       </c>
       <c r="EE12" t="inlineStr"/>
-      <c r="EF12" t="n">
-        <v>37.1</v>
-      </c>
+      <c r="EF12" t="inlineStr"/>
       <c r="EG12" t="n">
         <v>70.26666666666667</v>
       </c>
@@ -5019,9 +4581,7 @@
       <c r="EJ12" t="n">
         <v>7.193933</v>
       </c>
-      <c r="EK12" t="n">
-        <v>36.5</v>
-      </c>
+      <c r="EK12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -5041,9 +4601,7 @@
       <c r="E13" t="n">
         <v>3.806667</v>
       </c>
-      <c r="F13" t="n">
-        <v>39.9</v>
-      </c>
+      <c r="F13" t="inlineStr"/>
       <c r="G13" t="n">
         <v>71.73999999999999</v>
       </c>
@@ -5056,9 +4614,7 @@
       <c r="J13" t="n">
         <v>3.743333</v>
       </c>
-      <c r="K13" t="n">
-        <v>37.9</v>
-      </c>
+      <c r="K13" t="inlineStr"/>
       <c r="L13" t="n">
         <v>46.92666666666667</v>
       </c>
@@ -5078,9 +4634,7 @@
       <c r="T13" t="n">
         <v>16.4637</v>
       </c>
-      <c r="U13" t="n">
-        <v>43.175</v>
-      </c>
+      <c r="U13" t="inlineStr"/>
       <c r="V13" t="n">
         <v>73.3</v>
       </c>
@@ -5093,9 +4647,7 @@
       <c r="Y13" t="n">
         <v>3.988632</v>
       </c>
-      <c r="Z13" t="n">
-        <v>34.4</v>
-      </c>
+      <c r="Z13" t="inlineStr"/>
       <c r="AA13" t="n">
         <v>51.7</v>
       </c>
@@ -5106,9 +4658,7 @@
       <c r="AD13" t="n">
         <v>12.10333</v>
       </c>
-      <c r="AE13" t="n">
-        <v>41.3</v>
-      </c>
+      <c r="AE13" t="inlineStr"/>
       <c r="AF13" t="n">
         <v>73.09333333333332</v>
       </c>
@@ -5121,9 +4671,7 @@
       <c r="AI13" t="n">
         <v>3.606667</v>
       </c>
-      <c r="AJ13" t="n">
-        <v>38.725</v>
-      </c>
+      <c r="AJ13" t="inlineStr"/>
       <c r="AK13" t="n">
         <v>76.14666666666666</v>
       </c>
@@ -5136,9 +4684,7 @@
       <c r="AN13" t="n">
         <v>3.6561</v>
       </c>
-      <c r="AO13" t="n">
-        <v>39.275</v>
-      </c>
+      <c r="AO13" t="inlineStr"/>
       <c r="AP13" t="n">
         <v>76.96666666666667</v>
       </c>
@@ -5151,9 +4697,7 @@
       <c r="AS13" t="n">
         <v>3.686667</v>
       </c>
-      <c r="AT13" t="n">
-        <v>38.6</v>
-      </c>
+      <c r="AT13" t="inlineStr"/>
       <c r="AU13" t="n">
         <v>65.85000000000001</v>
       </c>
@@ -5166,9 +4710,7 @@
       <c r="AX13" t="n">
         <v>17.3896</v>
       </c>
-      <c r="AY13" t="n">
-        <v>40.75</v>
-      </c>
+      <c r="AY13" t="inlineStr"/>
       <c r="AZ13" t="n">
         <v>39.41666666666666</v>
       </c>
@@ -5179,9 +4721,7 @@
       <c r="BC13" t="n">
         <v>19.23333</v>
       </c>
-      <c r="BD13" t="n">
-        <v>42</v>
-      </c>
+      <c r="BD13" t="inlineStr"/>
       <c r="BE13" t="n">
         <v>44.45</v>
       </c>
@@ -5194,9 +4734,7 @@
       <c r="BH13" t="n">
         <v>7.133333</v>
       </c>
-      <c r="BI13" t="n">
-        <v>41.8</v>
-      </c>
+      <c r="BI13" t="inlineStr"/>
       <c r="BJ13" t="n">
         <v>70.43333333333334</v>
       </c>
@@ -5209,9 +4747,7 @@
       <c r="BM13" t="n">
         <v>6.136667</v>
       </c>
-      <c r="BN13" t="n">
-        <v>39.5</v>
-      </c>
+      <c r="BN13" t="inlineStr"/>
       <c r="BO13" t="n">
         <v>70.26666666666667</v>
       </c>
@@ -5224,9 +4760,7 @@
       <c r="BR13" t="n">
         <v>6.406667</v>
       </c>
-      <c r="BS13" t="n">
-        <v>39.125</v>
-      </c>
+      <c r="BS13" t="inlineStr"/>
       <c r="BT13" t="n">
         <v>51.35666666666666</v>
       </c>
@@ -5255,9 +4789,7 @@
         <v>5.548666</v>
       </c>
       <c r="CG13" t="inlineStr"/>
-      <c r="CH13" t="n">
-        <v>39.2</v>
-      </c>
+      <c r="CH13" t="inlineStr"/>
       <c r="CI13" t="n">
         <v>70.81</v>
       </c>
@@ -5270,9 +4802,7 @@
       <c r="CL13" t="n">
         <v>3.673333</v>
       </c>
-      <c r="CM13" t="n">
-        <v>32.3</v>
-      </c>
+      <c r="CM13" t="inlineStr"/>
       <c r="CN13" t="n">
         <v>72.13333333333333</v>
       </c>
@@ -5285,9 +4815,7 @@
       <c r="CQ13" t="n">
         <v>3.93</v>
       </c>
-      <c r="CR13" t="n">
-        <v>35.7</v>
-      </c>
+      <c r="CR13" t="inlineStr"/>
       <c r="CS13" t="n">
         <v>55.13333333333333</v>
       </c>
@@ -5298,9 +4826,7 @@
       <c r="CV13" t="n">
         <v>24.31</v>
       </c>
-      <c r="CW13" t="n">
-        <v>42.2</v>
-      </c>
+      <c r="CW13" t="inlineStr"/>
       <c r="CX13" t="n">
         <v>68.56999999999999</v>
       </c>
@@ -5313,9 +4839,7 @@
       <c r="DA13" t="n">
         <v>5.3</v>
       </c>
-      <c r="DB13" t="n">
-        <v>40.59999999999999</v>
-      </c>
+      <c r="DB13" t="inlineStr"/>
       <c r="DC13" t="n">
         <v>10.13666666666667</v>
       </c>
@@ -5326,9 +4850,7 @@
       <c r="DF13" t="n">
         <v>73.12</v>
       </c>
-      <c r="DG13" t="n">
-        <v>40.3</v>
-      </c>
+      <c r="DG13" t="inlineStr"/>
       <c r="DH13" t="n">
         <v>47.54333333333333</v>
       </c>
@@ -5348,9 +4870,7 @@
       </c>
       <c r="DO13" t="inlineStr"/>
       <c r="DP13" t="inlineStr"/>
-      <c r="DQ13" t="n">
-        <v>40.5</v>
-      </c>
+      <c r="DQ13" t="inlineStr"/>
       <c r="DR13" t="n">
         <v>66.72666666666667</v>
       </c>
@@ -5363,9 +4883,7 @@
       <c r="DU13" t="n">
         <v>5</v>
       </c>
-      <c r="DV13" t="n">
-        <v>38.525</v>
-      </c>
+      <c r="DV13" t="inlineStr"/>
       <c r="DW13" t="n">
         <v>78.38</v>
       </c>
@@ -5378,9 +4896,7 @@
       <c r="DZ13" t="n">
         <v>4.32</v>
       </c>
-      <c r="EA13" t="n">
-        <v>36.3</v>
-      </c>
+      <c r="EA13" t="inlineStr"/>
       <c r="EB13" t="inlineStr"/>
       <c r="EC13" t="n">
         <v>68437.60000000001</v>
@@ -5389,9 +4905,7 @@
         <v>3.618667</v>
       </c>
       <c r="EE13" t="inlineStr"/>
-      <c r="EF13" t="n">
-        <v>37.1</v>
-      </c>
+      <c r="EF13" t="inlineStr"/>
       <c r="EG13" t="n">
         <v>70.63333333333333</v>
       </c>
@@ -5404,9 +4918,7 @@
       <c r="EJ13" t="n">
         <v>7.56674</v>
       </c>
-      <c r="EK13" t="n">
-        <v>36.5</v>
-      </c>
+      <c r="EK13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
@@ -5426,9 +4938,7 @@
       <c r="E14" t="n">
         <v>3.64</v>
       </c>
-      <c r="F14" t="n">
-        <v>39.8</v>
-      </c>
+      <c r="F14" t="inlineStr"/>
       <c r="G14" t="n">
         <v>71.78666666666666</v>
       </c>
@@ -5441,9 +4951,7 @@
       <c r="J14" t="n">
         <v>3.556667</v>
       </c>
-      <c r="K14" t="n">
-        <v>37.9</v>
-      </c>
+      <c r="K14" t="inlineStr"/>
       <c r="L14" t="n">
         <v>48.58000000000001</v>
       </c>
@@ -5463,9 +4971,7 @@
       <c r="T14" t="n">
         <v>16.0117</v>
       </c>
-      <c r="U14" t="n">
-        <v>43.1</v>
-      </c>
+      <c r="U14" t="inlineStr"/>
       <c r="V14" t="n">
         <v>73.5</v>
       </c>
@@ -5478,9 +4984,7 @@
       <c r="Y14" t="n">
         <v>3.897252</v>
       </c>
-      <c r="Z14" t="n">
-        <v>34.4</v>
-      </c>
+      <c r="Z14" t="inlineStr"/>
       <c r="AA14" t="n">
         <v>53.5</v>
       </c>
@@ -5491,9 +4995,7 @@
       <c r="AD14" t="n">
         <v>14.46</v>
       </c>
-      <c r="AE14" t="n">
-        <v>41.3</v>
-      </c>
+      <c r="AE14" t="inlineStr"/>
       <c r="AF14" t="n">
         <v>73.18666666666667</v>
       </c>
@@ -5506,9 +5008,7 @@
       <c r="AI14" t="n">
         <v>3.456667</v>
       </c>
-      <c r="AJ14" t="n">
-        <v>38.5</v>
-      </c>
+      <c r="AJ14" t="inlineStr"/>
       <c r="AK14" t="n">
         <v>76.17</v>
       </c>
@@ -5521,9 +5021,7 @@
       <c r="AN14" t="n">
         <v>3.585467</v>
       </c>
-      <c r="AO14" t="n">
-        <v>39.3</v>
-      </c>
+      <c r="AO14" t="inlineStr"/>
       <c r="AP14" t="n">
         <v>77.10000000000001</v>
       </c>
@@ -5536,9 +5034,7 @@
       <c r="AS14" t="n">
         <v>3.533333</v>
       </c>
-      <c r="AT14" t="n">
-        <v>38.6</v>
-      </c>
+      <c r="AT14" t="inlineStr"/>
       <c r="AU14" t="n">
         <v>65.97</v>
       </c>
@@ -5551,9 +5047,7 @@
       <c r="AX14" t="n">
         <v>16.806</v>
       </c>
-      <c r="AY14" t="n">
-        <v>40.4</v>
-      </c>
+      <c r="AY14" t="inlineStr"/>
       <c r="AZ14" t="n">
         <v>41.74666666666667</v>
       </c>
@@ -5564,9 +5058,7 @@
       <c r="BC14" t="n">
         <v>19.16667</v>
       </c>
-      <c r="BD14" t="n">
-        <v>42</v>
-      </c>
+      <c r="BD14" t="inlineStr"/>
       <c r="BE14" t="n">
         <v>44.55333333333333</v>
       </c>
@@ -5579,9 +5071,7 @@
       <c r="BH14" t="n">
         <v>7.333333</v>
       </c>
-      <c r="BI14" t="n">
-        <v>41.8</v>
-      </c>
+      <c r="BI14" t="inlineStr"/>
       <c r="BJ14" t="n">
         <v>70.53333333333335</v>
       </c>
@@ -5594,9 +5084,7 @@
       <c r="BM14" t="n">
         <v>5.92</v>
       </c>
-      <c r="BN14" t="n">
-        <v>39.5</v>
-      </c>
+      <c r="BN14" t="inlineStr"/>
       <c r="BO14" t="n">
         <v>70.76666666666667</v>
       </c>
@@ -5609,9 +5097,7 @@
       <c r="BR14" t="n">
         <v>5.946667</v>
       </c>
-      <c r="BS14" t="n">
-        <v>39.1</v>
-      </c>
+      <c r="BS14" t="inlineStr"/>
       <c r="BT14" t="n">
         <v>52.33333333333334</v>
       </c>
@@ -5642,9 +5128,7 @@
         <v>5.098333</v>
       </c>
       <c r="CG14" t="inlineStr"/>
-      <c r="CH14" t="n">
-        <v>39.2</v>
-      </c>
+      <c r="CH14" t="inlineStr"/>
       <c r="CI14" t="n">
         <v>70.78666666666668</v>
       </c>
@@ -5657,9 +5141,7 @@
       <c r="CL14" t="n">
         <v>3.456667</v>
       </c>
-      <c r="CM14" t="n">
-        <v>32.3</v>
-      </c>
+      <c r="CM14" t="inlineStr"/>
       <c r="CN14" t="n">
         <v>72.76666666666667</v>
       </c>
@@ -5672,9 +5154,7 @@
       <c r="CQ14" t="n">
         <v>3.913333</v>
       </c>
-      <c r="CR14" t="n">
-        <v>35.7</v>
-      </c>
+      <c r="CR14" t="inlineStr"/>
       <c r="CS14" t="n">
         <v>58.26666666666667</v>
       </c>
@@ -5685,9 +5165,7 @@
       <c r="CV14" t="n">
         <v>24.25333</v>
       </c>
-      <c r="CW14" t="n">
-        <v>42.2</v>
-      </c>
+      <c r="CW14" t="inlineStr"/>
       <c r="CX14" t="n">
         <v>68.67999999999999</v>
       </c>
@@ -5700,9 +5178,7 @@
       <c r="DA14" t="n">
         <v>4.7</v>
       </c>
-      <c r="DB14" t="n">
-        <v>40.8</v>
-      </c>
+      <c r="DB14" t="inlineStr"/>
       <c r="DC14" t="n">
         <v>11.77333333333333</v>
       </c>
@@ -5713,9 +5189,7 @@
       <c r="DF14" t="n">
         <v>109.5333</v>
       </c>
-      <c r="DG14" t="n">
-        <v>40.3</v>
-      </c>
+      <c r="DG14" t="inlineStr"/>
       <c r="DH14" t="n">
         <v>48.99333333333333</v>
       </c>
@@ -5726,9 +5200,7 @@
       <c r="DK14" t="n">
         <v>21.53667</v>
       </c>
-      <c r="DL14" t="n">
-        <v>41.7</v>
-      </c>
+      <c r="DL14" t="inlineStr"/>
       <c r="DM14" t="n">
         <v>52.48333333333333</v>
       </c>
@@ -5737,9 +5209,7 @@
       </c>
       <c r="DO14" t="inlineStr"/>
       <c r="DP14" t="inlineStr"/>
-      <c r="DQ14" t="n">
-        <v>40.5</v>
-      </c>
+      <c r="DQ14" t="inlineStr"/>
       <c r="DR14" t="n">
         <v>66.89999999999999</v>
       </c>
@@ -5752,9 +5222,7 @@
       <c r="DU14" t="n">
         <v>4.58</v>
       </c>
-      <c r="DV14" t="n">
-        <v>38.6</v>
-      </c>
+      <c r="DV14" t="inlineStr"/>
       <c r="DW14" t="n">
         <v>78.06666666666666</v>
       </c>
@@ -5767,9 +5235,7 @@
       <c r="DZ14" t="n">
         <v>4.406667</v>
       </c>
-      <c r="EA14" t="n">
-        <v>36.3</v>
-      </c>
+      <c r="EA14" t="inlineStr"/>
       <c r="EB14" t="inlineStr"/>
       <c r="EC14" t="n">
         <v>66963</v>
@@ -5778,9 +5244,7 @@
         <v>3.052333</v>
       </c>
       <c r="EE14" t="inlineStr"/>
-      <c r="EF14" t="n">
-        <v>37.1</v>
-      </c>
+      <c r="EF14" t="inlineStr"/>
       <c r="EG14" t="n">
         <v>70.5</v>
       </c>
@@ -5793,9 +5257,7 @@
       <c r="EJ14" t="n">
         <v>7.56537</v>
       </c>
-      <c r="EK14" t="n">
-        <v>36.5</v>
-      </c>
+      <c r="EK14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
@@ -50350,6 +49812,563 @@
       </c>
       <c r="EK121" t="inlineStr"/>
     </row>
+    <row r="122">
+      <c r="A122" s="1" t="n">
+        <v>1995</v>
+      </c>
+      <c r="B122" t="inlineStr"/>
+      <c r="C122" t="inlineStr"/>
+      <c r="D122" t="inlineStr"/>
+      <c r="E122" t="inlineStr"/>
+      <c r="F122" t="n">
+        <v>40</v>
+      </c>
+      <c r="G122" t="inlineStr"/>
+      <c r="H122" t="inlineStr"/>
+      <c r="I122" t="inlineStr"/>
+      <c r="J122" t="inlineStr"/>
+      <c r="K122" t="n">
+        <v>37.8</v>
+      </c>
+      <c r="L122" t="inlineStr"/>
+      <c r="M122" t="inlineStr"/>
+      <c r="N122" t="inlineStr"/>
+      <c r="O122" t="inlineStr"/>
+      <c r="P122" t="inlineStr"/>
+      <c r="Q122" t="inlineStr"/>
+      <c r="R122" t="inlineStr"/>
+      <c r="S122" t="inlineStr"/>
+      <c r="T122" t="inlineStr"/>
+      <c r="U122" t="inlineStr"/>
+      <c r="V122" t="inlineStr"/>
+      <c r="W122" t="inlineStr"/>
+      <c r="X122" t="inlineStr"/>
+      <c r="Y122" t="inlineStr"/>
+      <c r="Z122" t="n">
+        <v>34.3</v>
+      </c>
+      <c r="AA122" t="inlineStr"/>
+      <c r="AB122" t="inlineStr"/>
+      <c r="AC122" t="inlineStr"/>
+      <c r="AD122" t="inlineStr"/>
+      <c r="AE122" t="inlineStr"/>
+      <c r="AF122" t="inlineStr"/>
+      <c r="AG122" t="inlineStr"/>
+      <c r="AH122" t="inlineStr"/>
+      <c r="AI122" t="inlineStr"/>
+      <c r="AJ122" t="n">
+        <v>36.9</v>
+      </c>
+      <c r="AK122" t="inlineStr"/>
+      <c r="AL122" t="inlineStr"/>
+      <c r="AM122" t="inlineStr"/>
+      <c r="AN122" t="inlineStr"/>
+      <c r="AO122" t="n">
+        <v>39.7</v>
+      </c>
+      <c r="AP122" t="inlineStr"/>
+      <c r="AQ122" t="inlineStr"/>
+      <c r="AR122" t="inlineStr"/>
+      <c r="AS122" t="inlineStr"/>
+      <c r="AT122" t="n">
+        <v>38.7</v>
+      </c>
+      <c r="AU122" t="inlineStr"/>
+      <c r="AV122" t="inlineStr"/>
+      <c r="AW122" t="inlineStr"/>
+      <c r="AX122" t="inlineStr"/>
+      <c r="AY122" t="n">
+        <v>42.3</v>
+      </c>
+      <c r="AZ122" t="inlineStr"/>
+      <c r="BA122" t="inlineStr"/>
+      <c r="BB122" t="inlineStr"/>
+      <c r="BC122" t="inlineStr"/>
+      <c r="BD122" t="inlineStr"/>
+      <c r="BE122" t="inlineStr"/>
+      <c r="BF122" t="inlineStr"/>
+      <c r="BG122" t="inlineStr"/>
+      <c r="BH122" t="inlineStr"/>
+      <c r="BI122" t="n">
+        <v>41.2</v>
+      </c>
+      <c r="BJ122" t="inlineStr"/>
+      <c r="BK122" t="inlineStr"/>
+      <c r="BL122" t="inlineStr"/>
+      <c r="BM122" t="inlineStr"/>
+      <c r="BN122" t="n">
+        <v>39.6</v>
+      </c>
+      <c r="BO122" t="inlineStr"/>
+      <c r="BP122" t="inlineStr"/>
+      <c r="BQ122" t="inlineStr"/>
+      <c r="BR122" t="inlineStr"/>
+      <c r="BS122" t="n">
+        <v>39.3</v>
+      </c>
+      <c r="BT122" t="inlineStr"/>
+      <c r="BU122" t="inlineStr"/>
+      <c r="BV122" t="inlineStr"/>
+      <c r="BW122" t="inlineStr"/>
+      <c r="BX122" t="inlineStr"/>
+      <c r="BY122" t="inlineStr"/>
+      <c r="BZ122" t="inlineStr"/>
+      <c r="CA122" t="inlineStr"/>
+      <c r="CB122" t="inlineStr"/>
+      <c r="CC122" t="inlineStr"/>
+      <c r="CD122" t="inlineStr"/>
+      <c r="CE122" t="inlineStr"/>
+      <c r="CF122" t="inlineStr"/>
+      <c r="CG122" t="inlineStr"/>
+      <c r="CH122" t="n">
+        <v>39.7</v>
+      </c>
+      <c r="CI122" t="inlineStr"/>
+      <c r="CJ122" t="inlineStr"/>
+      <c r="CK122" t="inlineStr"/>
+      <c r="CL122" t="inlineStr"/>
+      <c r="CM122" t="n">
+        <v>30.5</v>
+      </c>
+      <c r="CN122" t="inlineStr"/>
+      <c r="CO122" t="inlineStr"/>
+      <c r="CP122" t="inlineStr"/>
+      <c r="CQ122" t="inlineStr"/>
+      <c r="CR122" t="n">
+        <v>34.4</v>
+      </c>
+      <c r="CS122" t="inlineStr"/>
+      <c r="CT122" t="inlineStr"/>
+      <c r="CU122" t="inlineStr"/>
+      <c r="CV122" t="inlineStr"/>
+      <c r="CW122" t="inlineStr"/>
+      <c r="CX122" t="inlineStr"/>
+      <c r="CY122" t="inlineStr"/>
+      <c r="CZ122" t="inlineStr"/>
+      <c r="DA122" t="inlineStr"/>
+      <c r="DB122" t="n">
+        <v>41.6</v>
+      </c>
+      <c r="DC122" t="inlineStr"/>
+      <c r="DD122" t="inlineStr"/>
+      <c r="DE122" t="inlineStr"/>
+      <c r="DF122" t="inlineStr"/>
+      <c r="DG122" t="inlineStr"/>
+      <c r="DH122" t="inlineStr"/>
+      <c r="DI122" t="inlineStr"/>
+      <c r="DJ122" t="inlineStr"/>
+      <c r="DK122" t="inlineStr"/>
+      <c r="DL122" t="inlineStr"/>
+      <c r="DM122" t="inlineStr"/>
+      <c r="DN122" t="inlineStr"/>
+      <c r="DO122" t="inlineStr"/>
+      <c r="DP122" t="inlineStr"/>
+      <c r="DQ122" t="inlineStr"/>
+      <c r="DR122" t="inlineStr"/>
+      <c r="DS122" t="inlineStr"/>
+      <c r="DT122" t="inlineStr"/>
+      <c r="DU122" t="inlineStr"/>
+      <c r="DV122" t="n">
+        <v>38.3</v>
+      </c>
+      <c r="DW122" t="inlineStr"/>
+      <c r="DX122" t="inlineStr"/>
+      <c r="DY122" t="inlineStr"/>
+      <c r="DZ122" t="inlineStr"/>
+      <c r="EA122" t="n">
+        <v>34</v>
+      </c>
+      <c r="EB122" t="inlineStr"/>
+      <c r="EC122" t="inlineStr"/>
+      <c r="ED122" t="inlineStr"/>
+      <c r="EE122" t="inlineStr"/>
+      <c r="EF122" t="inlineStr"/>
+      <c r="EG122" t="inlineStr"/>
+      <c r="EH122" t="inlineStr"/>
+      <c r="EI122" t="inlineStr"/>
+      <c r="EJ122" t="inlineStr"/>
+      <c r="EK122" t="n">
+        <v>36.9</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="1" t="n">
+        <v>1996</v>
+      </c>
+      <c r="B123" t="inlineStr"/>
+      <c r="C123" t="inlineStr"/>
+      <c r="D123" t="inlineStr"/>
+      <c r="E123" t="inlineStr"/>
+      <c r="F123" t="n">
+        <v>39.8</v>
+      </c>
+      <c r="G123" t="inlineStr"/>
+      <c r="H123" t="inlineStr"/>
+      <c r="I123" t="inlineStr"/>
+      <c r="J123" t="inlineStr"/>
+      <c r="K123" t="n">
+        <v>37.8</v>
+      </c>
+      <c r="L123" t="inlineStr"/>
+      <c r="M123" t="inlineStr"/>
+      <c r="N123" t="inlineStr"/>
+      <c r="O123" t="inlineStr"/>
+      <c r="P123" t="inlineStr"/>
+      <c r="Q123" t="inlineStr"/>
+      <c r="R123" t="inlineStr"/>
+      <c r="S123" t="inlineStr"/>
+      <c r="T123" t="inlineStr"/>
+      <c r="U123" t="inlineStr"/>
+      <c r="V123" t="inlineStr"/>
+      <c r="W123" t="inlineStr"/>
+      <c r="X123" t="inlineStr"/>
+      <c r="Y123" t="inlineStr"/>
+      <c r="Z123" t="n">
+        <v>34</v>
+      </c>
+      <c r="AA123" t="inlineStr"/>
+      <c r="AB123" t="inlineStr"/>
+      <c r="AC123" t="inlineStr"/>
+      <c r="AD123" t="inlineStr"/>
+      <c r="AE123" t="inlineStr"/>
+      <c r="AF123" t="inlineStr"/>
+      <c r="AG123" t="inlineStr"/>
+      <c r="AH123" t="inlineStr"/>
+      <c r="AI123" t="inlineStr"/>
+      <c r="AJ123" t="n">
+        <v>37.6</v>
+      </c>
+      <c r="AK123" t="inlineStr"/>
+      <c r="AL123" t="inlineStr"/>
+      <c r="AM123" t="inlineStr"/>
+      <c r="AN123" t="inlineStr"/>
+      <c r="AO123" t="n">
+        <v>39.6</v>
+      </c>
+      <c r="AP123" t="inlineStr"/>
+      <c r="AQ123" t="inlineStr"/>
+      <c r="AR123" t="inlineStr"/>
+      <c r="AS123" t="inlineStr"/>
+      <c r="AT123" t="n">
+        <v>38.7</v>
+      </c>
+      <c r="AU123" t="inlineStr"/>
+      <c r="AV123" t="inlineStr"/>
+      <c r="AW123" t="inlineStr"/>
+      <c r="AX123" t="inlineStr"/>
+      <c r="AY123" t="n">
+        <v>41.9</v>
+      </c>
+      <c r="AZ123" t="inlineStr"/>
+      <c r="BA123" t="inlineStr"/>
+      <c r="BB123" t="inlineStr"/>
+      <c r="BC123" t="inlineStr"/>
+      <c r="BD123" t="n">
+        <v>41.2</v>
+      </c>
+      <c r="BE123" t="inlineStr"/>
+      <c r="BF123" t="inlineStr"/>
+      <c r="BG123" t="inlineStr"/>
+      <c r="BH123" t="inlineStr"/>
+      <c r="BI123" t="n">
+        <v>42.1</v>
+      </c>
+      <c r="BJ123" t="inlineStr"/>
+      <c r="BK123" t="inlineStr"/>
+      <c r="BL123" t="inlineStr"/>
+      <c r="BM123" t="inlineStr"/>
+      <c r="BN123" t="n">
+        <v>40.1</v>
+      </c>
+      <c r="BO123" t="inlineStr"/>
+      <c r="BP123" t="inlineStr"/>
+      <c r="BQ123" t="inlineStr"/>
+      <c r="BR123" t="inlineStr"/>
+      <c r="BS123" t="n">
+        <v>38.8</v>
+      </c>
+      <c r="BT123" t="inlineStr"/>
+      <c r="BU123" t="inlineStr"/>
+      <c r="BV123" t="inlineStr"/>
+      <c r="BW123" t="inlineStr"/>
+      <c r="BX123" t="inlineStr"/>
+      <c r="BY123" t="inlineStr"/>
+      <c r="BZ123" t="inlineStr"/>
+      <c r="CA123" t="inlineStr"/>
+      <c r="CB123" t="inlineStr"/>
+      <c r="CC123" t="inlineStr"/>
+      <c r="CD123" t="inlineStr"/>
+      <c r="CE123" t="inlineStr"/>
+      <c r="CF123" t="inlineStr"/>
+      <c r="CG123" t="inlineStr"/>
+      <c r="CH123" t="n">
+        <v>39.3</v>
+      </c>
+      <c r="CI123" t="inlineStr"/>
+      <c r="CJ123" t="inlineStr"/>
+      <c r="CK123" t="inlineStr"/>
+      <c r="CL123" t="inlineStr"/>
+      <c r="CM123" t="n">
+        <v>32.3</v>
+      </c>
+      <c r="CN123" t="inlineStr"/>
+      <c r="CO123" t="inlineStr"/>
+      <c r="CP123" t="inlineStr"/>
+      <c r="CQ123" t="inlineStr"/>
+      <c r="CR123" t="n">
+        <v>34.9</v>
+      </c>
+      <c r="CS123" t="inlineStr"/>
+      <c r="CT123" t="inlineStr"/>
+      <c r="CU123" t="inlineStr"/>
+      <c r="CV123" t="inlineStr"/>
+      <c r="CW123" t="inlineStr"/>
+      <c r="CX123" t="inlineStr"/>
+      <c r="CY123" t="inlineStr"/>
+      <c r="CZ123" t="inlineStr"/>
+      <c r="DA123" t="inlineStr"/>
+      <c r="DB123" t="n">
+        <v>40.8</v>
+      </c>
+      <c r="DC123" t="inlineStr"/>
+      <c r="DD123" t="inlineStr"/>
+      <c r="DE123" t="inlineStr"/>
+      <c r="DF123" t="inlineStr"/>
+      <c r="DG123" t="inlineStr"/>
+      <c r="DH123" t="inlineStr"/>
+      <c r="DI123" t="inlineStr"/>
+      <c r="DJ123" t="inlineStr"/>
+      <c r="DK123" t="inlineStr"/>
+      <c r="DL123" t="inlineStr"/>
+      <c r="DM123" t="inlineStr"/>
+      <c r="DN123" t="inlineStr"/>
+      <c r="DO123" t="inlineStr"/>
+      <c r="DP123" t="inlineStr"/>
+      <c r="DQ123" t="n">
+        <v>42.2</v>
+      </c>
+      <c r="DR123" t="inlineStr"/>
+      <c r="DS123" t="inlineStr"/>
+      <c r="DT123" t="inlineStr"/>
+      <c r="DU123" t="inlineStr"/>
+      <c r="DV123" t="n">
+        <v>38</v>
+      </c>
+      <c r="DW123" t="inlineStr"/>
+      <c r="DX123" t="inlineStr"/>
+      <c r="DY123" t="inlineStr"/>
+      <c r="DZ123" t="inlineStr"/>
+      <c r="EA123" t="n">
+        <v>34.4</v>
+      </c>
+      <c r="EB123" t="inlineStr"/>
+      <c r="EC123" t="inlineStr"/>
+      <c r="ED123" t="inlineStr"/>
+      <c r="EE123" t="inlineStr"/>
+      <c r="EF123" t="n">
+        <v>37</v>
+      </c>
+      <c r="EG123" t="inlineStr"/>
+      <c r="EH123" t="inlineStr"/>
+      <c r="EI123" t="inlineStr"/>
+      <c r="EJ123" t="inlineStr"/>
+      <c r="EK123" t="n">
+        <v>36.7</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="1" t="n">
+        <v>1997</v>
+      </c>
+      <c r="B124" t="inlineStr"/>
+      <c r="C124" t="inlineStr"/>
+      <c r="D124" t="inlineStr"/>
+      <c r="E124" t="inlineStr"/>
+      <c r="F124" t="n">
+        <v>40.2</v>
+      </c>
+      <c r="G124" t="inlineStr"/>
+      <c r="H124" t="inlineStr"/>
+      <c r="I124" t="inlineStr"/>
+      <c r="J124" t="inlineStr"/>
+      <c r="K124" t="n">
+        <v>37.9</v>
+      </c>
+      <c r="L124" t="inlineStr"/>
+      <c r="M124" t="inlineStr"/>
+      <c r="N124" t="inlineStr"/>
+      <c r="O124" t="inlineStr"/>
+      <c r="P124" t="inlineStr"/>
+      <c r="Q124" t="inlineStr"/>
+      <c r="R124" t="inlineStr"/>
+      <c r="S124" t="inlineStr"/>
+      <c r="T124" t="inlineStr"/>
+      <c r="U124" t="n">
+        <v>43.4</v>
+      </c>
+      <c r="V124" t="inlineStr"/>
+      <c r="W124" t="inlineStr"/>
+      <c r="X124" t="inlineStr"/>
+      <c r="Y124" t="inlineStr"/>
+      <c r="Z124" t="n">
+        <v>34.4</v>
+      </c>
+      <c r="AA124" t="inlineStr"/>
+      <c r="AB124" t="inlineStr"/>
+      <c r="AC124" t="inlineStr"/>
+      <c r="AD124" t="inlineStr"/>
+      <c r="AE124" t="n">
+        <v>41.3</v>
+      </c>
+      <c r="AF124" t="inlineStr"/>
+      <c r="AG124" t="inlineStr"/>
+      <c r="AH124" t="inlineStr"/>
+      <c r="AI124" t="inlineStr"/>
+      <c r="AJ124" t="n">
+        <v>39.4</v>
+      </c>
+      <c r="AK124" t="inlineStr"/>
+      <c r="AL124" t="inlineStr"/>
+      <c r="AM124" t="inlineStr"/>
+      <c r="AN124" t="inlineStr"/>
+      <c r="AO124" t="n">
+        <v>39.2</v>
+      </c>
+      <c r="AP124" t="inlineStr"/>
+      <c r="AQ124" t="inlineStr"/>
+      <c r="AR124" t="inlineStr"/>
+      <c r="AS124" t="inlineStr"/>
+      <c r="AT124" t="n">
+        <v>38.6</v>
+      </c>
+      <c r="AU124" t="inlineStr"/>
+      <c r="AV124" t="inlineStr"/>
+      <c r="AW124" t="inlineStr"/>
+      <c r="AX124" t="inlineStr"/>
+      <c r="AY124" t="n">
+        <v>41.8</v>
+      </c>
+      <c r="AZ124" t="inlineStr"/>
+      <c r="BA124" t="inlineStr"/>
+      <c r="BB124" t="inlineStr"/>
+      <c r="BC124" t="inlineStr"/>
+      <c r="BD124" t="n">
+        <v>42</v>
+      </c>
+      <c r="BE124" t="inlineStr"/>
+      <c r="BF124" t="inlineStr"/>
+      <c r="BG124" t="inlineStr"/>
+      <c r="BH124" t="inlineStr"/>
+      <c r="BI124" t="n">
+        <v>41.8</v>
+      </c>
+      <c r="BJ124" t="inlineStr"/>
+      <c r="BK124" t="inlineStr"/>
+      <c r="BL124" t="inlineStr"/>
+      <c r="BM124" t="inlineStr"/>
+      <c r="BN124" t="n">
+        <v>39.5</v>
+      </c>
+      <c r="BO124" t="inlineStr"/>
+      <c r="BP124" t="inlineStr"/>
+      <c r="BQ124" t="inlineStr"/>
+      <c r="BR124" t="inlineStr"/>
+      <c r="BS124" t="n">
+        <v>39.2</v>
+      </c>
+      <c r="BT124" t="inlineStr"/>
+      <c r="BU124" t="inlineStr"/>
+      <c r="BV124" t="inlineStr"/>
+      <c r="BW124" t="inlineStr"/>
+      <c r="BX124" t="inlineStr"/>
+      <c r="BY124" t="inlineStr"/>
+      <c r="BZ124" t="inlineStr"/>
+      <c r="CA124" t="inlineStr"/>
+      <c r="CB124" t="inlineStr"/>
+      <c r="CC124" t="inlineStr"/>
+      <c r="CD124" t="inlineStr"/>
+      <c r="CE124" t="inlineStr"/>
+      <c r="CF124" t="inlineStr"/>
+      <c r="CG124" t="inlineStr"/>
+      <c r="CH124" t="n">
+        <v>39.2</v>
+      </c>
+      <c r="CI124" t="inlineStr"/>
+      <c r="CJ124" t="inlineStr"/>
+      <c r="CK124" t="inlineStr"/>
+      <c r="CL124" t="inlineStr"/>
+      <c r="CM124" t="n">
+        <v>32.3</v>
+      </c>
+      <c r="CN124" t="inlineStr"/>
+      <c r="CO124" t="inlineStr"/>
+      <c r="CP124" t="inlineStr"/>
+      <c r="CQ124" t="inlineStr"/>
+      <c r="CR124" t="n">
+        <v>35.7</v>
+      </c>
+      <c r="CS124" t="inlineStr"/>
+      <c r="CT124" t="inlineStr"/>
+      <c r="CU124" t="inlineStr"/>
+      <c r="CV124" t="inlineStr"/>
+      <c r="CW124" t="n">
+        <v>42.2</v>
+      </c>
+      <c r="CX124" t="inlineStr"/>
+      <c r="CY124" t="inlineStr"/>
+      <c r="CZ124" t="inlineStr"/>
+      <c r="DA124" t="inlineStr"/>
+      <c r="DB124" t="n">
+        <v>40</v>
+      </c>
+      <c r="DC124" t="inlineStr"/>
+      <c r="DD124" t="inlineStr"/>
+      <c r="DE124" t="inlineStr"/>
+      <c r="DF124" t="inlineStr"/>
+      <c r="DG124" t="n">
+        <v>40.3</v>
+      </c>
+      <c r="DH124" t="inlineStr"/>
+      <c r="DI124" t="inlineStr"/>
+      <c r="DJ124" t="inlineStr"/>
+      <c r="DK124" t="inlineStr"/>
+      <c r="DL124" t="inlineStr"/>
+      <c r="DM124" t="inlineStr"/>
+      <c r="DN124" t="inlineStr"/>
+      <c r="DO124" t="inlineStr"/>
+      <c r="DP124" t="inlineStr"/>
+      <c r="DQ124" t="n">
+        <v>40.5</v>
+      </c>
+      <c r="DR124" t="inlineStr"/>
+      <c r="DS124" t="inlineStr"/>
+      <c r="DT124" t="inlineStr"/>
+      <c r="DU124" t="inlineStr"/>
+      <c r="DV124" t="n">
+        <v>38.3</v>
+      </c>
+      <c r="DW124" t="inlineStr"/>
+      <c r="DX124" t="inlineStr"/>
+      <c r="DY124" t="inlineStr"/>
+      <c r="DZ124" t="inlineStr"/>
+      <c r="EA124" t="n">
+        <v>36.3</v>
+      </c>
+      <c r="EB124" t="inlineStr"/>
+      <c r="EC124" t="inlineStr"/>
+      <c r="ED124" t="inlineStr"/>
+      <c r="EE124" t="inlineStr"/>
+      <c r="EF124" t="n">
+        <v>37.1</v>
+      </c>
+      <c r="EG124" t="inlineStr"/>
+      <c r="EH124" t="inlineStr"/>
+      <c r="EI124" t="inlineStr"/>
+      <c r="EJ124" t="inlineStr"/>
+      <c r="EK124" t="n">
+        <v>36.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>